<commit_message>
Working HTML- Input , minor bug fixies
working Server F_16_server.py (working download, upload, running, anbd output showing)  

and addtional over EXCEL with F_16.py (input data to change in input.xlsx)
</commit_message>
<xml_diff>
--- a/app/modules/common/AD/F16_input/DH_technology_cost.xlsx
+++ b/app/modules/common/AD/F16_input/DH_technology_cost.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nesa\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nesa\Desktop\Arbeit EEG\Hotmaps\Dispatch\app\modules\common\AD\F16_input\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2250" windowWidth="11970" windowHeight="4815" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="2250" windowWidth="11970" windowHeight="4815" firstSheet="1" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Parameter for Powerplants" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="98">
   <si>
     <t>el.Consumption</t>
   </si>
@@ -284,13 +284,37 @@
     <t>toatl_RF</t>
   </si>
   <si>
-    <t>Nan</t>
-  </si>
-  <si>
     <t>demand_factor</t>
   </si>
   <si>
     <t>total_demand</t>
+  </si>
+  <si>
+    <t>Interes Rate [0-1]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Demand </t>
+  </si>
+  <si>
+    <t>Temperature</t>
+  </si>
+  <si>
+    <t>Demand Scaling Factor [0-1]</t>
+  </si>
+  <si>
+    <t>Total Demand[ MWh]</t>
+  </si>
+  <si>
+    <t>Total Renewable Factor [0-1]</t>
+  </si>
+  <si>
+    <t>Threshold Temperature [Celsius]</t>
+  </si>
+  <si>
+    <t>Radiation</t>
+  </si>
+  <si>
+    <t>CO2 Price</t>
   </si>
 </sst>
 </file>
@@ -1943,7 +1967,7 @@
   <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1991,7 +2015,7 @@
         <v>18</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>87</v>
+        <v>76</v>
       </c>
       <c r="C4" s="4">
         <v>0.8</v>
@@ -2114,23 +2138,24 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P20" sqref="P20"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="5.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
@@ -2159,41 +2184,73 @@
         <v>86</v>
       </c>
       <c r="I1" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="J1" s="11" t="s">
         <v>88</v>
       </c>
-      <c r="J1" s="11" t="s">
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="10" t="s">
+        <v>97</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="D2" s="10" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="4">
+      <c r="E2" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="F2" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="G2" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="H2" s="10" t="s">
+        <v>94</v>
+      </c>
+      <c r="I2" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="J2" s="11" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="4">
         <v>25</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B3" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="C2" s="4">
-        <v>0</v>
-      </c>
-      <c r="D2" s="4">
+      <c r="C3" s="4">
+        <v>0</v>
+      </c>
+      <c r="D3" s="4">
         <v>0.5</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E3" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="F3" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="G2" s="4">
-        <v>0</v>
-      </c>
-      <c r="H2" s="4">
-        <v>0.5</v>
-      </c>
-      <c r="I2" s="4">
-        <v>1</v>
-      </c>
-      <c r="J2" s="15">
+      <c r="G3" s="4">
+        <v>0</v>
+      </c>
+      <c r="H3" s="4">
+        <v>0</v>
+      </c>
+      <c r="I3" s="4">
+        <v>1</v>
+      </c>
+      <c r="J3" s="15">
         <v>6000000</v>
       </c>
     </row>

</xml_diff>

<commit_message>
new features to bokeh server
-  invesment toggle button added
- "heat profile" - selection
- "electricity-price" selection
</commit_message>
<xml_diff>
--- a/app/modules/common/AD/F16_input/DH_technology_cost.xlsx
+++ b/app/modules/common/AD/F16_input/DH_technology_cost.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2250" windowWidth="11970" windowHeight="4815" firstSheet="1" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="2250" windowWidth="11970" windowHeight="4815"/>
   </bookViews>
   <sheets>
     <sheet name="Parameter for Powerplants" sheetId="1" r:id="rId1"/>
@@ -813,15 +813,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="37.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.5703125" customWidth="1"/>
+    <col min="4" max="4" width="17.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="25.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="25" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
@@ -1427,7 +1427,7 @@
         <v>2000</v>
       </c>
       <c r="K12" s="13">
-        <v>0.89999999999999991</v>
+        <v>0.9</v>
       </c>
       <c r="L12" s="13">
         <v>25</v>
@@ -2140,7 +2140,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Download and Upload feature fixed
TODO:
- upgrade to newer bokeh version
- Download with browser (JS)
- "compress" code ( rewrite redundant code)
</commit_message>
<xml_diff>
--- a/app/modules/common/AD/F16_input/DH_technology_cost.xlsx
+++ b/app/modules/common/AD/F16_input/DH_technology_cost.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="4950" windowWidth="11970" windowHeight="4815" firstSheet="1" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="5400" windowWidth="11970" windowHeight="4815"/>
   </bookViews>
   <sheets>
     <sheet name="Heat Generators" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="113">
   <si>
     <t>el.Consumption</t>
   </si>
@@ -265,21 +265,12 @@
     <t>P_co2</t>
   </si>
   <si>
-    <t>demand_th</t>
-  </si>
-  <si>
-    <t>heat_storage</t>
-  </si>
-  <si>
     <t>interest_rate</t>
   </si>
   <si>
     <t>radiation</t>
   </si>
   <si>
-    <t>temp</t>
-  </si>
-  <si>
     <t>threshold_heatpump</t>
   </si>
   <si>
@@ -295,12 +286,6 @@
     <t>Interes Rate [0-1]</t>
   </si>
   <si>
-    <t xml:space="preserve">Demand </t>
-  </si>
-  <si>
-    <t>Temperature</t>
-  </si>
-  <si>
     <t>Demand Scaling Factor [0-1]</t>
   </si>
   <si>
@@ -311,9 +296,6 @@
   </si>
   <si>
     <t>Threshold Temperature [Celsius]</t>
-  </si>
-  <si>
-    <t>Radiation</t>
   </si>
   <si>
     <t>CO2 Price</t>
@@ -892,7 +874,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P23"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
@@ -2040,13 +2022,13 @@
         <v>1</v>
       </c>
       <c r="B23" s="16" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="C23" s="16" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D23" s="16" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="E23" s="16">
         <v>0</v>
@@ -2082,7 +2064,7 @@
         <v>0</v>
       </c>
       <c r="P23" s="17" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
     </row>
   </sheetData>
@@ -2262,7 +2244,7 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="18" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B15" s="5">
         <v>0</v>
@@ -2278,27 +2260,23 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J3"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="22.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="22" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="20.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
         <v>79</v>
       </c>
@@ -2306,91 +2284,55 @@
         <v>80</v>
       </c>
       <c r="C1" s="11" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="D1" s="11" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="E1" s="11" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="F1" s="11" t="s">
-        <v>84</v>
-      </c>
-      <c r="G1" s="11" t="s">
         <v>85</v>
       </c>
-      <c r="H1" s="11" t="s">
+    </row>
+    <row r="2" spans="1:6" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="B2" s="11" t="s">
         <v>86</v>
       </c>
-      <c r="I1" s="11" t="s">
-        <v>87</v>
-      </c>
-      <c r="J1" s="11" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="11" t="s">
-        <v>97</v>
-      </c>
-      <c r="B2" s="11" t="s">
+      <c r="C2" s="11" t="s">
         <v>90</v>
-      </c>
-      <c r="C2" s="11" t="s">
-        <v>81</v>
       </c>
       <c r="D2" s="11" t="s">
         <v>89</v>
       </c>
       <c r="E2" s="11" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="F2" s="11" t="s">
-        <v>91</v>
-      </c>
-      <c r="G2" s="11" t="s">
-        <v>95</v>
-      </c>
-      <c r="H2" s="11" t="s">
-        <v>94</v>
-      </c>
-      <c r="I2" s="11" t="s">
-        <v>92</v>
-      </c>
-      <c r="J2" s="11" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>25</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>76</v>
+      <c r="B3" s="2">
+        <v>0.5</v>
       </c>
       <c r="C3" s="2">
         <v>0</v>
       </c>
       <c r="D3" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="G3" s="2">
-        <v>0</v>
-      </c>
-      <c r="H3" s="2">
-        <v>0</v>
-      </c>
-      <c r="I3" s="2">
-        <v>1</v>
-      </c>
-      <c r="J3" s="9">
+        <v>0</v>
+      </c>
+      <c r="E3" s="2">
+        <v>1</v>
+      </c>
+      <c r="F3" s="9">
         <v>6000000</v>
       </c>
     </row>
@@ -2403,7 +2345,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+    <sheetView topLeftCell="E1" workbookViewId="0">
       <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
@@ -2423,34 +2365,34 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="B1" s="14" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="C1" s="14" t="s">
+        <v>97</v>
+      </c>
+      <c r="D1" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="E1" s="14" t="s">
+        <v>107</v>
+      </c>
+      <c r="F1" s="14" t="s">
+        <v>108</v>
+      </c>
+      <c r="G1" s="14" t="s">
         <v>103</v>
       </c>
-      <c r="D1" s="14" t="s">
-        <v>101</v>
-      </c>
-      <c r="E1" s="14" t="s">
-        <v>113</v>
-      </c>
-      <c r="F1" s="14" t="s">
-        <v>114</v>
-      </c>
-      <c r="G1" s="14" t="s">
+      <c r="H1" s="14" t="s">
         <v>109</v>
       </c>
-      <c r="H1" s="14" t="s">
-        <v>115</v>
-      </c>
       <c r="I1" s="14" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="J1" s="14" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2458,36 +2400,36 @@
         <v>48</v>
       </c>
       <c r="B2" s="14" t="s">
+        <v>100</v>
+      </c>
+      <c r="C2" s="19" t="s">
+        <v>111</v>
+      </c>
+      <c r="D2" s="14" t="s">
+        <v>96</v>
+      </c>
+      <c r="E2" s="14" t="s">
+        <v>98</v>
+      </c>
+      <c r="F2" s="14" t="s">
+        <v>99</v>
+      </c>
+      <c r="G2" s="14" t="s">
+        <v>102</v>
+      </c>
+      <c r="H2" s="14" t="s">
         <v>106</v>
       </c>
-      <c r="C2" s="19" t="s">
-        <v>117</v>
-      </c>
-      <c r="D2" s="14" t="s">
-        <v>102</v>
-      </c>
-      <c r="E2" s="14" t="s">
-        <v>104</v>
-      </c>
-      <c r="F2" s="14" t="s">
-        <v>105</v>
-      </c>
-      <c r="G2" s="14" t="s">
-        <v>108</v>
-      </c>
-      <c r="H2" s="14" t="s">
+      <c r="I2" s="14" t="s">
         <v>112</v>
       </c>
-      <c r="I2" s="14" t="s">
-        <v>118</v>
-      </c>
       <c r="J2" s="14" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="B3" s="4">
         <v>1000</v>

</xml_diff>

<commit_message>
Fix Heat Storage Bug
TODO:
- upgrade to newer bokeh version
- Download with browser (JS)
- "compress" code ( rewrite redundant code)
</commit_message>
<xml_diff>
--- a/app/modules/common/AD/F16_input/DH_technology_cost.xlsx
+++ b/app/modules/common/AD/F16_input/DH_technology_cost.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="5400" windowWidth="11970" windowHeight="4815"/>
+    <workbookView xWindow="0" yWindow="5850" windowWidth="11970" windowHeight="4815" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Heat Generators" sheetId="1" r:id="rId1"/>
@@ -874,7 +874,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+    <sheetView topLeftCell="F1" workbookViewId="0">
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
@@ -2345,8 +2345,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J3"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2432,7 +2432,7 @@
         <v>105</v>
       </c>
       <c r="B3" s="4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="C3" s="4">
         <v>300</v>

</xml_diff>

<commit_message>
Several imrovments at must run and heat storage
</commit_message>
<xml_diff>
--- a/app/modules/common/AD/F16_input/DH_technology_cost.xlsx
+++ b/app/modules/common/AD/F16_input/DH_technology_cost.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18326"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19330"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nesa\Desktop\Arbeit EEG\Hotmaps\Dispatch\app\modules\common\AD\F16_input\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\david\Documents\GitKraken\Dispatch\app\modules\common\AD\F16_input\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{E8BFDC57-A2DD-4FAE-9583-BB87F8A8339F}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="6750" windowWidth="11970" windowHeight="4815" firstSheet="1" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="6756" windowWidth="11976" windowHeight="4812" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Heat Generators" sheetId="1" r:id="rId1"/>
@@ -23,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="115">
   <si>
     <t>el.Consumption</t>
   </si>
@@ -283,9 +284,6 @@
     <t>total_demand</t>
   </si>
   <si>
-    <t>Interes Rate [0-1]</t>
-  </si>
-  <si>
     <t>Demand Scaling Factor [0-1]</t>
   </si>
   <si>
@@ -362,12 +360,21 @@
   </si>
   <si>
     <t>unloading efficiency</t>
+  </si>
+  <si>
+    <t>MR</t>
+  </si>
+  <si>
+    <t>must run [0-1]</t>
+  </si>
+  <si>
+    <t>Interest Rate [0-1]</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -480,7 +487,7 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
@@ -530,6 +537,13 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -871,33 +885,33 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P23"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:Q23"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="Q2" sqref="Q2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="37.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="37.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="25.109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="25" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="29.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="27.7109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="18.7109375" style="1" customWidth="1"/>
-    <col min="15" max="15" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="48.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="29.44140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.5546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="27.6640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="18.6640625" style="1" customWidth="1"/>
+    <col min="15" max="15" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="48.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="11" t="s">
         <v>45</v>
       </c>
@@ -946,8 +960,11 @@
       <c r="P1" s="11" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="2" spans="1:16" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="Q1" s="20" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" s="13" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="11" t="s">
         <v>45</v>
       </c>
@@ -996,8 +1013,11 @@
       <c r="P2" s="12" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q2" s="21" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
         <v>1</v>
       </c>
@@ -1047,8 +1067,11 @@
         <f>CONCATENATE(A3," ",B3," ",C3)</f>
         <v>heat boiler natural gas</v>
       </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q3" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
         <v>1</v>
       </c>
@@ -1098,8 +1121,11 @@
         <f t="shared" ref="P4:P22" si="0">CONCATENATE(A4," ",B4," ",C4)</f>
         <v>heat boiler wood chips</v>
       </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q4" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
         <v>1</v>
       </c>
@@ -1149,8 +1175,11 @@
         <f t="shared" si="0"/>
         <v>heat boiler wood pellets</v>
       </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q5" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
         <v>1</v>
       </c>
@@ -1200,8 +1229,11 @@
         <f t="shared" si="0"/>
         <v>heat boiler straw</v>
       </c>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q6" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
         <v>1</v>
       </c>
@@ -1251,8 +1283,11 @@
         <f t="shared" si="0"/>
         <v>heat waste treatment waste</v>
       </c>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q7" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
         <v>1</v>
       </c>
@@ -1302,8 +1337,11 @@
         <f t="shared" si="0"/>
         <v>heat boiler electricity</v>
       </c>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q8" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
         <v>1</v>
       </c>
@@ -1353,8 +1391,11 @@
         <f t="shared" si="0"/>
         <v>heat comp. heat pump ambient heat</v>
       </c>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q9" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A10" s="7" t="s">
         <v>1</v>
       </c>
@@ -1404,8 +1445,11 @@
         <f t="shared" si="0"/>
         <v>heat comp. heat pump waste heat 20°</v>
       </c>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q10" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="s">
         <v>1</v>
       </c>
@@ -1455,8 +1499,11 @@
         <f t="shared" si="0"/>
         <v>heat comp. heat pump waste heat 40°</v>
       </c>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q11" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A12" s="7" t="s">
         <v>1</v>
       </c>
@@ -1506,8 +1553,11 @@
         <f t="shared" si="0"/>
         <v>heat abs. heat pump various</v>
       </c>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q12" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A13" s="7" t="s">
         <v>2</v>
       </c>
@@ -1557,8 +1607,11 @@
         <f t="shared" si="0"/>
         <v>CHP stirling engine gas. Biomass</v>
       </c>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q13" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A14" s="7" t="s">
         <v>2</v>
       </c>
@@ -1608,8 +1661,11 @@
         <f t="shared" si="0"/>
         <v>CHP steam turbine (medium) wood chips</v>
       </c>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q14" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A15" s="7" t="s">
         <v>2</v>
       </c>
@@ -1659,8 +1715,11 @@
         <f t="shared" si="0"/>
         <v>CHP steam turbine (small) wood chips</v>
       </c>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q15" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A16" s="7" t="s">
         <v>2</v>
       </c>
@@ -1710,8 +1769,11 @@
         <f t="shared" si="0"/>
         <v>CHP steam turbine (medium) straw</v>
       </c>
-    </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q16" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A17" s="7" t="s">
         <v>2</v>
       </c>
@@ -1761,8 +1823,11 @@
         <f t="shared" si="0"/>
         <v>CHP steam turbine (small) straw</v>
       </c>
-    </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q17" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A18" s="7" t="s">
         <v>2</v>
       </c>
@@ -1812,8 +1877,11 @@
         <f t="shared" si="0"/>
         <v>CHP waste treatment waste</v>
       </c>
-    </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q18" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A19" s="7" t="s">
         <v>2</v>
       </c>
@@ -1863,8 +1931,11 @@
         <f t="shared" si="0"/>
         <v>CHP spark ignition natural gas</v>
       </c>
-    </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q19" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A20" s="7" t="s">
         <v>2</v>
       </c>
@@ -1914,8 +1985,11 @@
         <f t="shared" si="0"/>
         <v>CHP spark ignition gas. Biomass</v>
       </c>
-    </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q20" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A21" s="7" t="s">
         <v>2</v>
       </c>
@@ -1965,8 +2039,11 @@
         <f t="shared" si="0"/>
         <v>CHP CC gas turbine/ steam extraction turbine gas/oil</v>
       </c>
-    </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q21" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A22" s="7" t="s">
         <v>2</v>
       </c>
@@ -2016,19 +2093,22 @@
         <f t="shared" si="0"/>
         <v>CHP CC gas turbine/ back-pressure turbine gas/oil</v>
       </c>
-    </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q22" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A23" s="16" t="s">
         <v>1</v>
       </c>
       <c r="B23" s="16" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C23" s="16" t="s">
         <v>81</v>
       </c>
       <c r="D23" s="16" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E23" s="16">
         <v>0</v>
@@ -2064,7 +2144,10 @@
         <v>0</v>
       </c>
       <c r="P23" s="17" t="s">
-        <v>106</v>
+        <v>105</v>
+      </c>
+      <c r="Q23" s="17">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -2074,21 +2157,21 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C15" sqref="A15:C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.140625" customWidth="1"/>
-    <col min="2" max="2" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.109375" customWidth="1"/>
+    <col min="2" max="2" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="14" t="s">
         <v>70</v>
       </c>
@@ -2099,7 +2182,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="2" spans="1:3" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="14" t="s">
         <v>60</v>
       </c>
@@ -2110,7 +2193,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>19</v>
       </c>
@@ -2121,7 +2204,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>18</v>
       </c>
@@ -2132,7 +2215,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>23</v>
       </c>
@@ -2143,7 +2226,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>24</v>
       </c>
@@ -2154,7 +2237,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
         <v>13</v>
       </c>
@@ -2165,7 +2248,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>16</v>
       </c>
@@ -2176,7 +2259,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
         <v>22</v>
       </c>
@@ -2187,7 +2270,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
         <v>17</v>
       </c>
@@ -2198,7 +2281,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
         <v>20</v>
       </c>
@@ -2209,7 +2292,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
         <v>21</v>
       </c>
@@ -2220,7 +2303,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
         <v>14</v>
       </c>
@@ -2231,7 +2314,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
         <v>15</v>
       </c>
@@ -2242,7 +2325,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" s="18" t="s">
         <v>81</v>
       </c>
@@ -2259,24 +2342,24 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="11" t="s">
         <v>79</v>
       </c>
@@ -2296,27 +2379,27 @@
         <v>85</v>
       </c>
     </row>
-    <row r="2" spans="1:6" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="11" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B2" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="E2" s="11" t="s">
         <v>86</v>
       </c>
-      <c r="C2" s="11" t="s">
-        <v>90</v>
-      </c>
-      <c r="D2" s="11" t="s">
-        <v>89</v>
-      </c>
-      <c r="E2" s="11" t="s">
+      <c r="F2" s="11" t="s">
         <v>87</v>
       </c>
-      <c r="F2" s="11" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>25</v>
       </c>
@@ -2342,94 +2425,94 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:J3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="30.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="51.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="51.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="30.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="51.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="51.109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.33203125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="B1" s="14" t="s">
+        <v>100</v>
+      </c>
+      <c r="C1" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="D1" s="14" t="s">
+        <v>94</v>
+      </c>
+      <c r="E1" s="14" t="s">
+        <v>102</v>
+      </c>
+      <c r="F1" s="14" t="s">
+        <v>103</v>
+      </c>
+      <c r="G1" s="14" t="s">
+        <v>99</v>
+      </c>
+      <c r="H1" s="14" t="s">
+        <v>104</v>
+      </c>
+      <c r="I1" s="14" t="s">
         <v>92</v>
       </c>
-      <c r="B1" s="14" t="s">
-        <v>101</v>
-      </c>
-      <c r="C1" s="14" t="s">
-        <v>96</v>
-      </c>
-      <c r="D1" s="14" t="s">
-        <v>95</v>
-      </c>
-      <c r="E1" s="14" t="s">
-        <v>103</v>
-      </c>
-      <c r="F1" s="14" t="s">
-        <v>104</v>
-      </c>
-      <c r="G1" s="14" t="s">
-        <v>100</v>
-      </c>
-      <c r="H1" s="14" t="s">
-        <v>105</v>
-      </c>
-      <c r="I1" s="14" t="s">
+      <c r="J1" s="14" t="s">
         <v>93</v>
       </c>
-      <c r="J1" s="14" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="14" t="s">
         <v>48</v>
       </c>
       <c r="B2" s="14" t="s">
+        <v>96</v>
+      </c>
+      <c r="C2" s="19" t="s">
+        <v>107</v>
+      </c>
+      <c r="D2" s="14" t="s">
+        <v>108</v>
+      </c>
+      <c r="E2" s="14" t="s">
+        <v>109</v>
+      </c>
+      <c r="F2" s="14" t="s">
+        <v>111</v>
+      </c>
+      <c r="G2" s="14" t="s">
+        <v>98</v>
+      </c>
+      <c r="H2" s="14" t="s">
+        <v>110</v>
+      </c>
+      <c r="I2" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="J2" s="14" t="s">
         <v>97</v>
       </c>
-      <c r="C2" s="19" t="s">
-        <v>108</v>
-      </c>
-      <c r="D2" s="14" t="s">
-        <v>109</v>
-      </c>
-      <c r="E2" s="14" t="s">
-        <v>110</v>
-      </c>
-      <c r="F2" s="14" t="s">
-        <v>112</v>
-      </c>
-      <c r="G2" s="14" t="s">
-        <v>99</v>
-      </c>
-      <c r="H2" s="14" t="s">
-        <v>111</v>
-      </c>
-      <c r="I2" s="14" t="s">
-        <v>107</v>
-      </c>
-      <c r="J2" s="14" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B3" s="4">
         <v>0</v>

</xml_diff>

<commit_message>
new features: added visual options for adding heat generators
also new output visualizations added :
 - heat storage level is now an extra plot 
 - also the ranking of technologies (CHP) has been changed
       
TODO:
- adding Heat Generators to Data Table
- adding new features also for the heat storages
- rewrite redundant code (specially F16_server.py)
- migate to newest bokeh version
- maybe delete initial table -> then the page dont look overloaded -> user friendly
- CHP production characteristic formulated as a line
  (maybe defining  realistic production range with
   binary variables )

- download files via Browser (JavaScript)

Versions of Main Packages:
    bokeh=='0.12.10', pandas=='0.22.0',
    numpy=='1.14.0, pyomo=='5.5.0'
</commit_message>
<xml_diff>
--- a/app/modules/common/AD/F16_input/DH_technology_cost.xlsx
+++ b/app/modules/common/AD/F16_input/DH_technology_cost.xlsx
@@ -1,22 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19330"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18326"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\david\Documents\GitKraken\Dispatch\app\modules\common\AD\F16_input\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nesa\Desktop\Arbeit EEG\Hotmaps\Dispatch\app\modules\common\AD\F16_input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{E8BFDC57-A2DD-4FAE-9583-BB87F8A8339F}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="6756" windowWidth="11976" windowHeight="4812" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="9900" windowWidth="11970" windowHeight="4815"/>
   </bookViews>
   <sheets>
     <sheet name="Heat Generators" sheetId="1" r:id="rId1"/>
     <sheet name="prices and emmision factors" sheetId="2" r:id="rId2"/>
     <sheet name="financal and other parameteres" sheetId="3" r:id="rId3"/>
     <sheet name="Heat Storage" sheetId="4" r:id="rId4"/>
+    <sheet name="Techologies" sheetId="9" r:id="rId5"/>
+    <sheet name="Heat Pump1" sheetId="5" r:id="rId6"/>
+    <sheet name="Heat Pump2" sheetId="6" r:id="rId7"/>
+    <sheet name="Heat Pump3" sheetId="7" r:id="rId8"/>
+    <sheet name="Heat Pump4" sheetId="8" r:id="rId9"/>
   </sheets>
   <calcPr calcId="162913"/>
   <fileRecoveryPr autoRecover="0"/>
@@ -24,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="136">
   <si>
     <t>el.Consumption</t>
   </si>
@@ -369,13 +373,76 @@
   </si>
   <si>
     <t>Interest Rate [0-1]</t>
+  </si>
+  <si>
+    <t>COP</t>
+  </si>
+  <si>
+    <t>70°C</t>
+  </si>
+  <si>
+    <t>75°C</t>
+  </si>
+  <si>
+    <t>80°C</t>
+  </si>
+  <si>
+    <t>85°C</t>
+  </si>
+  <si>
+    <t>90°C</t>
+  </si>
+  <si>
+    <t>95°C</t>
+  </si>
+  <si>
+    <t>40°C</t>
+  </si>
+  <si>
+    <t>45°C</t>
+  </si>
+  <si>
+    <t>50°C</t>
+  </si>
+  <si>
+    <t>55°C</t>
+  </si>
+  <si>
+    <t>60°C</t>
+  </si>
+  <si>
+    <t>65°C</t>
+  </si>
+  <si>
+    <t>heat pump</t>
+  </si>
+  <si>
+    <t>Power to Heat</t>
+  </si>
+  <si>
+    <t>Geo Thermal</t>
+  </si>
+  <si>
+    <t>heat pump - High Temperature -Geo Thermal (60°C)</t>
+  </si>
+  <si>
+    <t>heat pump - Default</t>
+  </si>
+  <si>
+    <t>heat pump - River 5°C</t>
+  </si>
+  <si>
+    <t>heat pump - River 10°C</t>
+  </si>
+  <si>
+    <t>Techologies</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -411,6 +478,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="6">
@@ -487,7 +560,7 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
@@ -543,6 +616,16 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -885,33 +968,33 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q23"/>
   <sheetViews>
-    <sheetView topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="Q2" sqref="Q2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="37.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="25.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="37.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="25.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="25" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.88671875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="29.44140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="19.6640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="20.33203125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="8.5546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="27.6640625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="18.6640625" style="1" customWidth="1"/>
-    <col min="15" max="15" width="15.109375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="48.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="29.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="27.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="18.7109375" style="1" customWidth="1"/>
+    <col min="15" max="15" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="48.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
         <v>45</v>
       </c>
@@ -964,7 +1047,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="2" spans="1:17" s="13" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:17" s="13" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
         <v>45</v>
       </c>
@@ -1017,7 +1100,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>1</v>
       </c>
@@ -1071,7 +1154,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>1</v>
       </c>
@@ -1125,7 +1208,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>1</v>
       </c>
@@ -1179,7 +1262,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>1</v>
       </c>
@@ -1233,7 +1316,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>1</v>
       </c>
@@ -1287,7 +1370,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>1</v>
       </c>
@@ -1341,7 +1424,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>1</v>
       </c>
@@ -1395,7 +1478,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>1</v>
       </c>
@@ -1449,7 +1532,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>1</v>
       </c>
@@ -1503,7 +1586,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>1</v>
       </c>
@@ -1557,7 +1640,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>2</v>
       </c>
@@ -1611,7 +1694,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
         <v>2</v>
       </c>
@@ -1665,7 +1748,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
         <v>2</v>
       </c>
@@ -1719,7 +1802,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
         <v>2</v>
       </c>
@@ -1773,7 +1856,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
         <v>2</v>
       </c>
@@ -1827,7 +1910,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
         <v>2</v>
       </c>
@@ -1881,7 +1964,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
         <v>2</v>
       </c>
@@ -1935,7 +2018,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
         <v>2</v>
       </c>
@@ -1989,7 +2072,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
         <v>2</v>
       </c>
@@ -2043,7 +2126,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
         <v>2</v>
       </c>
@@ -2097,7 +2180,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A23" s="16" t="s">
         <v>1</v>
       </c>
@@ -2157,21 +2240,21 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C15" sqref="A15:C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.109375" customWidth="1"/>
-    <col min="2" max="2" width="20.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.140625" customWidth="1"/>
+    <col min="2" max="2" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="15" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="s">
         <v>70</v>
       </c>
@@ -2182,7 +2265,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="2" spans="1:3" s="15" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
         <v>60</v>
       </c>
@@ -2193,7 +2276,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>19</v>
       </c>
@@ -2204,7 +2287,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>18</v>
       </c>
@@ -2215,7 +2298,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>23</v>
       </c>
@@ -2226,7 +2309,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>24</v>
       </c>
@@ -2237,7 +2320,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>13</v>
       </c>
@@ -2248,7 +2331,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>16</v>
       </c>
@@ -2259,7 +2342,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>22</v>
       </c>
@@ -2270,7 +2353,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>17</v>
       </c>
@@ -2281,7 +2364,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>20</v>
       </c>
@@ -2292,7 +2375,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>21</v>
       </c>
@@ -2303,7 +2386,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>14</v>
       </c>
@@ -2314,7 +2397,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>15</v>
       </c>
@@ -2325,7 +2408,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="18" t="s">
         <v>81</v>
       </c>
@@ -2342,24 +2425,24 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.88671875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="15" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
         <v>79</v>
       </c>
@@ -2379,7 +2462,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="2" spans="1:6" s="15" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
         <v>90</v>
       </c>
@@ -2399,7 +2482,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>25</v>
       </c>
@@ -2425,28 +2508,28 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="30.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.44140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="51.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="51.109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="30.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="51.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="51.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.28515625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="s">
         <v>91</v>
       </c>
@@ -2478,7 +2561,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
         <v>48</v>
       </c>
@@ -2510,7 +2593,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>101</v>
       </c>
@@ -2546,4 +2629,872 @@
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="25.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="25" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" s="22" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" s="22" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" s="22" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" s="22" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" s="26" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" s="22" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" s="25" t="s">
+        <v>130</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="24" t="s">
+        <v>115</v>
+      </c>
+      <c r="B2" t="s">
+        <v>116</v>
+      </c>
+      <c r="C2" t="s">
+        <v>117</v>
+      </c>
+      <c r="D2" t="s">
+        <v>118</v>
+      </c>
+      <c r="E2" t="s">
+        <v>119</v>
+      </c>
+      <c r="F2" t="s">
+        <v>120</v>
+      </c>
+      <c r="G2" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>122</v>
+      </c>
+      <c r="B3">
+        <v>48.67</v>
+      </c>
+      <c r="C3">
+        <v>44.95</v>
+      </c>
+      <c r="D3">
+        <v>39.14</v>
+      </c>
+      <c r="E3">
+        <v>31.73</v>
+      </c>
+      <c r="F3">
+        <v>16.170000000000002</v>
+      </c>
+      <c r="G3">
+        <v>9.49</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>123</v>
+      </c>
+      <c r="B4">
+        <v>40.96</v>
+      </c>
+      <c r="C4">
+        <v>36.49</v>
+      </c>
+      <c r="D4">
+        <v>30.97</v>
+      </c>
+      <c r="E4">
+        <v>24.14</v>
+      </c>
+      <c r="F4">
+        <v>16.46</v>
+      </c>
+      <c r="G4">
+        <v>10.210000000000001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>124</v>
+      </c>
+      <c r="B5">
+        <v>23.95</v>
+      </c>
+      <c r="C5">
+        <v>21.28</v>
+      </c>
+      <c r="D5">
+        <v>33.729999999999997</v>
+      </c>
+      <c r="E5">
+        <v>25.89</v>
+      </c>
+      <c r="F5">
+        <v>15</v>
+      </c>
+      <c r="G5">
+        <v>10.02</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>125</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>13.11</v>
+      </c>
+      <c r="D6">
+        <v>17.41</v>
+      </c>
+      <c r="E6">
+        <v>15.05</v>
+      </c>
+      <c r="F6">
+        <v>11.67</v>
+      </c>
+      <c r="G6">
+        <v>9.0399999999999991</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>126</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>7.57</v>
+      </c>
+      <c r="E7">
+        <v>8.0299999999999994</v>
+      </c>
+      <c r="F7">
+        <v>8.07</v>
+      </c>
+      <c r="G7">
+        <v>7.28</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>127</v>
+      </c>
+      <c r="B8">
+        <v>0</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>5.86</v>
+      </c>
+      <c r="F8">
+        <v>4.96</v>
+      </c>
+      <c r="G8">
+        <v>4.72</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>116</v>
+      </c>
+      <c r="B9">
+        <v>0</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <v>5.33</v>
+      </c>
+      <c r="G9">
+        <v>4.3099999999999996</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="23" t="s">
+        <v>115</v>
+      </c>
+      <c r="B2" t="s">
+        <v>116</v>
+      </c>
+      <c r="C2" t="s">
+        <v>117</v>
+      </c>
+      <c r="D2" t="s">
+        <v>118</v>
+      </c>
+      <c r="E2" t="s">
+        <v>119</v>
+      </c>
+      <c r="F2" t="s">
+        <v>120</v>
+      </c>
+      <c r="G2" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="23" t="s">
+        <v>122</v>
+      </c>
+      <c r="B3">
+        <v>5.01</v>
+      </c>
+      <c r="C3">
+        <v>4.54</v>
+      </c>
+      <c r="D3">
+        <v>4.18</v>
+      </c>
+      <c r="E3">
+        <v>3.86</v>
+      </c>
+      <c r="F3">
+        <v>3.57</v>
+      </c>
+      <c r="G3">
+        <v>3.27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="23" t="s">
+        <v>123</v>
+      </c>
+      <c r="B4">
+        <v>4.76</v>
+      </c>
+      <c r="C4">
+        <v>4.33</v>
+      </c>
+      <c r="D4">
+        <v>3.99</v>
+      </c>
+      <c r="E4">
+        <v>3.66</v>
+      </c>
+      <c r="F4">
+        <v>3.45</v>
+      </c>
+      <c r="G4">
+        <v>3.15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="23" t="s">
+        <v>124</v>
+      </c>
+      <c r="B5">
+        <v>4.6399999999999997</v>
+      </c>
+      <c r="C5">
+        <v>4.2300000000000004</v>
+      </c>
+      <c r="D5">
+        <v>3.9</v>
+      </c>
+      <c r="E5">
+        <v>3.55</v>
+      </c>
+      <c r="F5">
+        <v>3.33</v>
+      </c>
+      <c r="G5">
+        <v>3.09</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="23" t="s">
+        <v>125</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>4.08</v>
+      </c>
+      <c r="D6">
+        <v>3.71</v>
+      </c>
+      <c r="E6">
+        <v>3.42</v>
+      </c>
+      <c r="F6">
+        <v>3.2</v>
+      </c>
+      <c r="G6">
+        <v>2.98</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="23" t="s">
+        <v>126</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>3.6</v>
+      </c>
+      <c r="E7">
+        <v>3.33</v>
+      </c>
+      <c r="F7">
+        <v>3.04</v>
+      </c>
+      <c r="G7">
+        <v>2.87</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="23" t="s">
+        <v>127</v>
+      </c>
+      <c r="B8">
+        <v>0</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>3.18</v>
+      </c>
+      <c r="F8">
+        <v>2.81</v>
+      </c>
+      <c r="G8">
+        <v>2.65</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="23" t="s">
+        <v>116</v>
+      </c>
+      <c r="B9">
+        <v>0</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <v>2.8</v>
+      </c>
+      <c r="G9">
+        <v>2.46</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>115</v>
+      </c>
+      <c r="B2" t="s">
+        <v>116</v>
+      </c>
+      <c r="C2" t="s">
+        <v>117</v>
+      </c>
+      <c r="D2" t="s">
+        <v>118</v>
+      </c>
+      <c r="E2" t="s">
+        <v>119</v>
+      </c>
+      <c r="F2" t="s">
+        <v>120</v>
+      </c>
+      <c r="G2" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>122</v>
+      </c>
+      <c r="B3">
+        <v>3.08</v>
+      </c>
+      <c r="C3">
+        <v>2.95</v>
+      </c>
+      <c r="D3">
+        <v>2.83</v>
+      </c>
+      <c r="E3">
+        <v>2.72</v>
+      </c>
+      <c r="F3">
+        <v>2.61</v>
+      </c>
+      <c r="G3">
+        <v>2.5299999999999998</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>123</v>
+      </c>
+      <c r="B4">
+        <v>2.99</v>
+      </c>
+      <c r="C4">
+        <v>2.88</v>
+      </c>
+      <c r="D4">
+        <v>2.77</v>
+      </c>
+      <c r="E4">
+        <v>2.66</v>
+      </c>
+      <c r="F4">
+        <v>2.57</v>
+      </c>
+      <c r="G4">
+        <v>2.48</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>124</v>
+      </c>
+      <c r="B5">
+        <v>2.94</v>
+      </c>
+      <c r="C5">
+        <v>2.81</v>
+      </c>
+      <c r="D5">
+        <v>2.71</v>
+      </c>
+      <c r="E5">
+        <v>2.61</v>
+      </c>
+      <c r="F5">
+        <v>2.5099999999999998</v>
+      </c>
+      <c r="G5">
+        <v>2.4300000000000002</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>125</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>2.75</v>
+      </c>
+      <c r="D6">
+        <v>2.64</v>
+      </c>
+      <c r="E6">
+        <v>2.54</v>
+      </c>
+      <c r="F6">
+        <v>2.4500000000000002</v>
+      </c>
+      <c r="G6">
+        <v>2.38</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>126</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>2.58</v>
+      </c>
+      <c r="E7">
+        <v>2.4900000000000002</v>
+      </c>
+      <c r="F7">
+        <v>2.4</v>
+      </c>
+      <c r="G7">
+        <v>2.3199999999999998</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>127</v>
+      </c>
+      <c r="B8">
+        <v>0</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>2.4300000000000002</v>
+      </c>
+      <c r="F8">
+        <v>2.34</v>
+      </c>
+      <c r="G8">
+        <v>2.27</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>116</v>
+      </c>
+      <c r="B9">
+        <v>0</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <v>2.29</v>
+      </c>
+      <c r="G9">
+        <v>2.2200000000000002</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G32" sqref="G32"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>115</v>
+      </c>
+      <c r="B2" t="s">
+        <v>116</v>
+      </c>
+      <c r="C2" t="s">
+        <v>117</v>
+      </c>
+      <c r="D2" t="s">
+        <v>118</v>
+      </c>
+      <c r="E2" t="s">
+        <v>119</v>
+      </c>
+      <c r="F2" t="s">
+        <v>120</v>
+      </c>
+      <c r="G2" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>122</v>
+      </c>
+      <c r="B3">
+        <v>3.41</v>
+      </c>
+      <c r="C3">
+        <v>3.25</v>
+      </c>
+      <c r="D3">
+        <v>3.11</v>
+      </c>
+      <c r="E3">
+        <v>2.99</v>
+      </c>
+      <c r="F3">
+        <v>2.87</v>
+      </c>
+      <c r="G3">
+        <v>2.77</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>123</v>
+      </c>
+      <c r="B4">
+        <v>3.32</v>
+      </c>
+      <c r="C4">
+        <v>3.18</v>
+      </c>
+      <c r="D4">
+        <v>3.04</v>
+      </c>
+      <c r="E4">
+        <v>2.92</v>
+      </c>
+      <c r="F4">
+        <v>2.82</v>
+      </c>
+      <c r="G4">
+        <v>2.71</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>124</v>
+      </c>
+      <c r="B5">
+        <v>3.26</v>
+      </c>
+      <c r="C5">
+        <v>3.11</v>
+      </c>
+      <c r="D5">
+        <v>2.98</v>
+      </c>
+      <c r="E5">
+        <v>2.86</v>
+      </c>
+      <c r="F5">
+        <v>2.76</v>
+      </c>
+      <c r="G5">
+        <v>2.66</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>125</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>3.04</v>
+      </c>
+      <c r="D6">
+        <v>2.91</v>
+      </c>
+      <c r="E6">
+        <v>2.8</v>
+      </c>
+      <c r="F6">
+        <v>2.7</v>
+      </c>
+      <c r="G6">
+        <v>2.6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>126</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>2.85</v>
+      </c>
+      <c r="E7">
+        <v>2.74</v>
+      </c>
+      <c r="F7">
+        <v>2.64</v>
+      </c>
+      <c r="G7">
+        <v>2.5499999999999998</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>127</v>
+      </c>
+      <c r="B8">
+        <v>0</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>2.67</v>
+      </c>
+      <c r="F8">
+        <v>2.58</v>
+      </c>
+      <c r="G8">
+        <v>2.4900000000000002</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>116</v>
+      </c>
+      <c r="B9">
+        <v>0</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <v>2.52</v>
+      </c>
+      <c r="G9">
+        <v>2.4300000000000002</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Download fix ( working JS Code) , download data  and graphocs after run
TODO: routine to clean up conten of the static folder
</commit_message>
<xml_diff>
--- a/app/modules/common/AD/F16_input/DH_technology_cost.xlsx
+++ b/app/modules/common/AD/F16_input/DH_technology_cost.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="9900" windowWidth="11970" windowHeight="4815" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="10350" windowWidth="11970" windowHeight="4815" firstSheet="3" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Heat Generators" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="134">
   <si>
     <t>el.Consumption</t>
   </si>
@@ -415,12 +415,6 @@
   </si>
   <si>
     <t>heat pump</t>
-  </si>
-  <si>
-    <t>Power to Heat</t>
-  </si>
-  <si>
-    <t>Geo Thermal</t>
   </si>
   <si>
     <t>heat pump - High Temperature -Geo Thermal (60°C)</t>
@@ -971,7 +965,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
@@ -2633,10 +2627,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A8"/>
+  <dimension ref="A1:A6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2646,7 +2640,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="25" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
@@ -2672,16 +2666,6 @@
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" s="26" t="s">
         <v>105</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" s="22" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" s="25" t="s">
-        <v>130</v>
       </c>
     </row>
   </sheetData>
@@ -2699,7 +2683,7 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -2901,7 +2885,7 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -3103,7 +3087,7 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -3307,7 +3291,7 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Bug fix astype or int values and load solved data
</commit_message>
<xml_diff>
--- a/app/modules/common/AD/F16_input/DH_technology_cost.xlsx
+++ b/app/modules/common/AD/F16_input/DH_technology_cost.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18326"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nesa\Desktop\Arbeit EEG\Hotmaps\Dispatch\app\modules\common\AD\F16_input\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="10350" windowWidth="11970" windowHeight="4815"/>
+    <workbookView xWindow="0" yWindow="10350" windowWidth="11970" windowHeight="4815" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Heat Generators" sheetId="1" r:id="rId1"/>
@@ -22,7 +17,7 @@
     <sheet name="Heat Pump3" sheetId="7" r:id="rId8"/>
     <sheet name="Heat Pump4" sheetId="8" r:id="rId9"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="145621"/>
   <fileRecoveryPr autoRecover="0"/>
 </workbook>
 </file>
@@ -447,7 +442,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -652,9 +647,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Larissa">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -692,9 +687,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Larissa">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -727,26 +722,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -779,26 +757,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Larissa">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -974,8 +935,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E31" sqref="E31"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2431,8 +2392,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2493,7 +2454,7 @@
         <v>0.5</v>
       </c>
       <c r="C3" s="2">
-        <v>0</v>
+        <v>-20</v>
       </c>
       <c r="D3" s="2">
         <v>0</v>

</xml_diff>

<commit_message>
Changing label names for units
</commit_message>
<xml_diff>
--- a/app/modules/common/AD/F16_input/DH_technology_cost.xlsx
+++ b/app/modules/common/AD/F16_input/DH_technology_cost.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="10350" windowWidth="11970" windowHeight="4815" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="10350" windowWidth="11970" windowHeight="4815" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Heat Generators" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="136">
   <si>
     <t>el.Consumption</t>
   </si>
@@ -231,9 +231,6 @@
     <t>em</t>
   </si>
   <si>
-    <t>emission factor</t>
-  </si>
-  <si>
     <t>prices(EUR/MWh)</t>
   </si>
   <si>
@@ -291,15 +288,9 @@
     <t>Total Demand[ MWh]</t>
   </si>
   <si>
-    <t>Total Renewable Factor [0-1]</t>
-  </si>
-  <si>
     <t>Threshold Temperature [Celsius]</t>
   </si>
   <si>
-    <t>CO2 Price</t>
-  </si>
-  <si>
     <t>hs_name</t>
   </si>
   <si>
@@ -321,9 +312,6 @@
     <t>Life Time [a]</t>
   </si>
   <si>
-    <t>Invesment costs for additional storage capacity  [€/MW]</t>
-  </si>
-  <si>
     <t>IK_cap_hs</t>
   </si>
   <si>
@@ -339,15 +327,9 @@
     <t>n_turb_hs</t>
   </si>
   <si>
-    <t>IK_pump_hs</t>
-  </si>
-  <si>
     <t>Solar Thermal</t>
   </si>
   <si>
-    <t>OPEX fix [€/MWa]</t>
-  </si>
-  <si>
     <t>maximum unloading power  [MW]</t>
   </si>
   <si>
@@ -357,9 +339,6 @@
     <t>loading efficiency</t>
   </si>
   <si>
-    <t>Invesment costs for additional loading power  [€/MW]</t>
-  </si>
-  <si>
     <t>unloading efficiency</t>
   </si>
   <si>
@@ -442,6 +421,21 @@
   </si>
   <si>
     <t>CHP-SE</t>
+  </si>
+  <si>
+    <t>Minimum Renewable Factor [0-1]</t>
+  </si>
+  <si>
+    <t>emission factor [tCO2/MWh]</t>
+  </si>
+  <si>
+    <t>CO2 Price [EUR/tC02]</t>
+  </si>
+  <si>
+    <t>OPEX fix [€/MWha]</t>
+  </si>
+  <si>
+    <t>Invesment costs for additional storage capacity  [€/MWh]</t>
   </si>
 </sst>
 </file>
@@ -1005,7 +999,7 @@
         <v>45</v>
       </c>
       <c r="C1" s="11" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D1" s="11" t="s">
         <v>58</v>
@@ -1014,13 +1008,13 @@
         <v>64</v>
       </c>
       <c r="F1" s="11" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G1" s="11" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H1" s="11" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="I1" s="11" t="s">
         <v>60</v>
@@ -1035,19 +1029,19 @@
         <v>61</v>
       </c>
       <c r="M1" s="11" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="N1" s="11" t="s">
         <v>65</v>
       </c>
       <c r="O1" s="11" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="P1" s="11" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="Q1" s="20" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
     </row>
     <row r="2" spans="1:17" s="13" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -1100,7 +1094,7 @@
         <v>47</v>
       </c>
       <c r="Q2" s="21" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
@@ -1645,7 +1639,7 @@
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
       <c r="B13" s="7" t="s">
         <v>6</v>
@@ -1699,7 +1693,7 @@
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" s="22" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="B14" s="7" t="s">
         <v>7</v>
@@ -1753,7 +1747,7 @@
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" s="22" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="B15" s="7" t="s">
         <v>8</v>
@@ -1807,7 +1801,7 @@
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" s="22" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="B16" s="7" t="s">
         <v>7</v>
@@ -1861,7 +1855,7 @@
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17" s="22" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="B17" s="7" t="s">
         <v>8</v>
@@ -1915,7 +1909,7 @@
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18" s="22" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="B18" s="7" t="s">
         <v>3</v>
@@ -1969,7 +1963,7 @@
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
       <c r="B19" s="7" t="s">
         <v>9</v>
@@ -2023,7 +2017,7 @@
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
       <c r="B20" s="7" t="s">
         <v>9</v>
@@ -2077,7 +2071,7 @@
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A21" s="22" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="B21" s="7" t="s">
         <v>10</v>
@@ -2131,7 +2125,7 @@
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
       <c r="B22" s="7" t="s">
         <v>11</v>
@@ -2188,13 +2182,13 @@
         <v>1</v>
       </c>
       <c r="B23" s="16" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="C23" s="16" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D23" s="16" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="E23" s="16">
         <v>0</v>
@@ -2230,7 +2224,7 @@
         <v>0</v>
       </c>
       <c r="P23" s="17" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="Q23" s="17">
         <v>0</v>
@@ -2247,7 +2241,7 @@
   <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C15" sqref="A15:C15"/>
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2259,10 +2253,10 @@
   <sheetData>
     <row r="1" spans="1:3" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="s">
+        <v>68</v>
+      </c>
+      <c r="B1" s="14" t="s">
         <v>69</v>
-      </c>
-      <c r="B1" s="14" t="s">
-        <v>70</v>
       </c>
       <c r="C1" s="14" t="s">
         <v>66</v>
@@ -2273,10 +2267,10 @@
         <v>59</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C2" s="14" t="s">
-        <v>67</v>
+        <v>132</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -2295,7 +2289,7 @@
         <v>17</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C4" s="2">
         <v>0.8</v>
@@ -2413,7 +2407,7 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="18" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B15" s="5">
         <v>0</v>
@@ -2432,7 +2426,7 @@
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2447,42 +2441,42 @@
   <sheetData>
     <row r="1" spans="1:6" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="B1" s="11" t="s">
         <v>78</v>
       </c>
-      <c r="B1" s="11" t="s">
-        <v>79</v>
-      </c>
       <c r="C1" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="D1" s="11" t="s">
         <v>81</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="E1" s="11" t="s">
         <v>82</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="F1" s="11" t="s">
         <v>83</v>
-      </c>
-      <c r="F1" s="11" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="2" spans="1:6" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
-        <v>89</v>
+        <v>133</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D2" s="11" t="s">
-        <v>87</v>
+        <v>131</v>
       </c>
       <c r="E2" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="F2" s="11" t="s">
         <v>85</v>
-      </c>
-      <c r="F2" s="11" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -2512,102 +2506,95 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J3"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="23.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="32" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="30.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="18.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="51.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="51.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="52.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="s">
+        <v>87</v>
+      </c>
+      <c r="B1" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="C1" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="D1" s="14" t="s">
         <v>90</v>
       </c>
-      <c r="B1" s="14" t="s">
-        <v>99</v>
-      </c>
-      <c r="C1" s="14" t="s">
+      <c r="E1" s="14" t="s">
+        <v>97</v>
+      </c>
+      <c r="F1" s="14" t="s">
+        <v>98</v>
+      </c>
+      <c r="G1" s="14" t="s">
         <v>94</v>
       </c>
-      <c r="D1" s="14" t="s">
-        <v>93</v>
-      </c>
-      <c r="E1" s="14" t="s">
-        <v>101</v>
-      </c>
-      <c r="F1" s="14" t="s">
-        <v>102</v>
-      </c>
-      <c r="G1" s="14" t="s">
-        <v>98</v>
-      </c>
       <c r="H1" s="14" t="s">
-        <v>103</v>
+        <v>88</v>
       </c>
       <c r="I1" s="14" t="s">
-        <v>91</v>
-      </c>
-      <c r="J1" s="14" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
         <v>47</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="C2" s="19" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="D2" s="14" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="E2" s="14" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="F2" s="14" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="G2" s="14" t="s">
-        <v>97</v>
+        <v>135</v>
       </c>
       <c r="H2" s="14" t="s">
-        <v>109</v>
+        <v>134</v>
       </c>
       <c r="I2" s="14" t="s">
-        <v>105</v>
-      </c>
-      <c r="J2" s="14" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
-        <v>100</v>
-      </c>
       <c r="B3" s="4">
         <v>0</v>
       </c>
       <c r="C3" s="4">
-        <v>300</v>
+        <v>80</v>
       </c>
       <c r="D3" s="4">
-        <v>300</v>
+        <v>80</v>
       </c>
       <c r="E3" s="4">
         <v>0.95</v>
@@ -2619,12 +2606,9 @@
         <v>60</v>
       </c>
       <c r="H3" s="4">
-        <v>250</v>
+        <v>10000</v>
       </c>
       <c r="I3" s="4">
-        <v>10000</v>
-      </c>
-      <c r="J3" s="4">
         <v>25</v>
       </c>
     </row>
@@ -2638,7 +2622,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
@@ -2649,12 +2633,12 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="25" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="22" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
@@ -2664,12 +2648,12 @@
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="22" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
@@ -2679,22 +2663,22 @@
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" s="22" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" s="22" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" s="22" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" s="22" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
     </row>
   </sheetData>
@@ -2712,35 +2696,35 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="24" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="B2" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="C2" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="D2" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="E2" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="F2" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="G2" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="B3">
         <v>48.67</v>
@@ -2763,7 +2747,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="B4">
         <v>40.96</v>
@@ -2786,7 +2770,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
       <c r="B5">
         <v>23.95</v>
@@ -2809,7 +2793,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -2832,7 +2816,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="B7">
         <v>0</v>
@@ -2855,7 +2839,7 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="B8">
         <v>0</v>
@@ -2878,7 +2862,7 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="B9">
         <v>0</v>
@@ -2914,35 +2898,35 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="23" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="B2" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="C2" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="D2" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="E2" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="F2" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="G2" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="23" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="B3">
         <v>5.01</v>
@@ -2965,7 +2949,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="23" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="B4">
         <v>4.76</v>
@@ -2988,7 +2972,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="23" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
       <c r="B5">
         <v>4.6399999999999997</v>
@@ -3011,7 +2995,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="23" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -3034,7 +3018,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="23" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="B7">
         <v>0</v>
@@ -3057,7 +3041,7 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="23" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="B8">
         <v>0</v>
@@ -3080,7 +3064,7 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="23" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="B9">
         <v>0</v>
@@ -3116,35 +3100,35 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="B2" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="C2" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="D2" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="E2" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="F2" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="G2" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="B3">
         <v>3.08</v>
@@ -3167,7 +3151,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="B4">
         <v>2.99</v>
@@ -3190,7 +3174,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
       <c r="B5">
         <v>2.94</v>
@@ -3213,7 +3197,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -3236,7 +3220,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="B7">
         <v>0</v>
@@ -3259,7 +3243,7 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="B8">
         <v>0</v>
@@ -3282,7 +3266,7 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="B9">
         <v>0</v>
@@ -3320,35 +3304,35 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="B2" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="C2" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="D2" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="E2" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="F2" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="G2" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="B3">
         <v>3.41</v>
@@ -3371,7 +3355,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="B4">
         <v>3.32</v>
@@ -3394,7 +3378,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
       <c r="B5">
         <v>3.26</v>
@@ -3417,7 +3401,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -3440,7 +3424,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="B7">
         <v>0</v>
@@ -3463,7 +3447,7 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="B8">
         <v>0</v>
@@ -3486,7 +3470,7 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="B9">
         <v>0</v>

</xml_diff>

<commit_message>
Input For Heat Storage Losses added
</commit_message>
<xml_diff>
--- a/app/modules/common/AD/F16_input/DH_technology_cost.xlsx
+++ b/app/modules/common/AD/F16_input/DH_technology_cost.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="138">
   <si>
     <t>el.Consumption</t>
   </si>
@@ -432,10 +432,16 @@
     <t>CO2 Price [EUR/tC02]</t>
   </si>
   <si>
-    <t>OPEX fix [€/MWha]</t>
-  </si>
-  <si>
     <t>Invesment costs for additional storage capacity  [€/MWh]</t>
+  </si>
+  <si>
+    <t>cap_losse_hs</t>
+  </si>
+  <si>
+    <t>Hourly Stoarge Losses [%]</t>
+  </si>
+  <si>
+    <t>OPEX fix [€/MWh]</t>
   </si>
 </sst>
 </file>
@@ -2506,26 +2512,27 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="23.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="32" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="30.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="52.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.5703125" customWidth="1"/>
+    <col min="4" max="4" width="32" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="30.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="52.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="s">
         <v>87</v>
       </c>
@@ -2533,57 +2540,63 @@
         <v>95</v>
       </c>
       <c r="C1" s="14" t="s">
+        <v>135</v>
+      </c>
+      <c r="D1" s="14" t="s">
         <v>91</v>
       </c>
-      <c r="D1" s="14" t="s">
+      <c r="E1" s="14" t="s">
         <v>90</v>
       </c>
-      <c r="E1" s="14" t="s">
+      <c r="F1" s="14" t="s">
         <v>97</v>
       </c>
-      <c r="F1" s="14" t="s">
+      <c r="G1" s="14" t="s">
         <v>98</v>
       </c>
-      <c r="G1" s="14" t="s">
+      <c r="H1" s="14" t="s">
         <v>94</v>
       </c>
-      <c r="H1" s="14" t="s">
+      <c r="I1" s="14" t="s">
         <v>88</v>
       </c>
-      <c r="I1" s="14" t="s">
+      <c r="J1" s="14" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
         <v>47</v>
       </c>
       <c r="B2" s="14" t="s">
         <v>92</v>
       </c>
-      <c r="C2" s="19" t="s">
+      <c r="C2" s="14" t="s">
+        <v>136</v>
+      </c>
+      <c r="D2" s="19" t="s">
         <v>100</v>
       </c>
-      <c r="D2" s="14" t="s">
+      <c r="E2" s="14" t="s">
         <v>101</v>
       </c>
-      <c r="E2" s="14" t="s">
+      <c r="F2" s="14" t="s">
         <v>102</v>
       </c>
-      <c r="F2" s="14" t="s">
+      <c r="G2" s="14" t="s">
         <v>103</v>
-      </c>
-      <c r="G2" s="14" t="s">
-        <v>135</v>
       </c>
       <c r="H2" s="14" t="s">
         <v>134</v>
       </c>
       <c r="I2" s="14" t="s">
+        <v>137</v>
+      </c>
+      <c r="J2" s="14" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>96</v>
       </c>
@@ -2591,24 +2604,27 @@
         <v>0</v>
       </c>
       <c r="C3" s="4">
-        <v>80</v>
+        <v>1</v>
       </c>
       <c r="D3" s="4">
         <v>80</v>
       </c>
       <c r="E3" s="4">
+        <v>80</v>
+      </c>
+      <c r="F3" s="4">
         <v>0.95</v>
       </c>
-      <c r="F3" s="4">
+      <c r="G3" s="4">
         <v>0.98</v>
       </c>
-      <c r="G3" s="4">
+      <c r="H3" s="4">
         <v>60</v>
       </c>
-      <c r="H3" s="4">
+      <c r="I3" s="4">
         <v>10000</v>
       </c>
-      <c r="I3" s="4">
+      <c r="J3" s="4">
         <v>25</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add input file in scenario output folder structure
</commit_message>
<xml_diff>
--- a/app/modules/common/AD/F16_input/DH_technology_cost.xlsx
+++ b/app/modules/common/AD/F16_input/DH_technology_cost.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18326"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20342"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nesa\Desktop\Arbeit EEG\Hotmaps\Dispatch\app\modules\common\AD\F16_input\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hasani\Documents\Workplace\Dispatch\app\modules\common\AD\F16_input\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE6438F7-FE6F-4094-B6DA-EFEE0C4D6AE5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="10350" windowWidth="11970" windowHeight="4815" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="10350" windowWidth="11970" windowHeight="4815" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Heat Generators" sheetId="1" r:id="rId1"/>
@@ -22,7 +23,7 @@
     <sheet name="Heat Pump3" sheetId="7" r:id="rId8"/>
     <sheet name="Heat Pump4" sheetId="8" r:id="rId9"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <fileRecoveryPr autoRecover="0"/>
 </workbook>
 </file>
@@ -447,7 +448,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -971,11 +972,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1489,7 +1490,7 @@
         <v>4</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D10" s="7" t="s">
         <v>31</v>
@@ -1529,7 +1530,7 @@
       </c>
       <c r="P10" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>heat comp. heat pump waste heat 20°</v>
+        <v>heat comp. heat pump electricity</v>
       </c>
       <c r="Q10" s="22">
         <v>0</v>
@@ -1543,7 +1544,7 @@
         <v>4</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D11" s="7" t="s">
         <v>32</v>
@@ -1583,7 +1584,7 @@
       </c>
       <c r="P11" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>heat comp. heat pump waste heat 40°</v>
+        <v>heat comp. heat pump electricity</v>
       </c>
       <c r="Q11" s="22">
         <v>0</v>
@@ -1597,7 +1598,7 @@
         <v>5</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="D12" s="7" t="s">
         <v>33</v>
@@ -1637,7 +1638,7 @@
       </c>
       <c r="P12" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>heat abs. heat pump various</v>
+        <v>heat abs. heat pump electricity</v>
       </c>
       <c r="Q12" s="22">
         <v>0</v>
@@ -2243,11 +2244,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2320,7 +2321,7 @@
         <v>47</v>
       </c>
       <c r="C6" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -2331,7 +2332,7 @@
         <v>30</v>
       </c>
       <c r="C7" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -2428,7 +2429,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2511,11 +2512,11 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2616,7 +2617,7 @@
         <v>0.95</v>
       </c>
       <c r="G3" s="4">
-        <v>0.52</v>
+        <v>0.95</v>
       </c>
       <c r="H3" s="4">
         <v>60</v>
@@ -2635,7 +2636,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:A10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2703,7 +2704,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -2905,7 +2906,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -3107,7 +3108,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -3309,7 +3310,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>

<commit_message>
some bug fixies and cleaning default data
</commit_message>
<xml_diff>
--- a/app/modules/common/AD/F16_input/DH_technology_cost.xlsx
+++ b/app/modules/common/AD/F16_input/DH_technology_cost.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hasani\Documents\Workplace\Dispatch\app\modules\common\AD\F16_input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{513A80D5-5BB3-4F68-B7A0-5F166413BCB6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00E8E80D-F3FF-4709-9028-E2A328F32943}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="10350" windowWidth="11970" windowHeight="4815" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,6 +22,7 @@
     <sheet name="Heat Pump2" sheetId="6" r:id="rId7"/>
     <sheet name="Heat Pump3" sheetId="7" r:id="rId8"/>
     <sheet name="Heat Pump4" sheetId="8" r:id="rId9"/>
+    <sheet name="CHP-SE" sheetId="10" r:id="rId10"/>
   </sheets>
   <calcPr calcId="191029"/>
   <fileRecoveryPr autoRecover="0"/>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="144">
   <si>
     <t>boiler</t>
   </si>
@@ -61,24 +62,9 @@
     <t>electricity</t>
   </si>
   <si>
-    <t>ambient heat</t>
-  </si>
-  <si>
-    <t>waste heat 20°</t>
-  </si>
-  <si>
-    <t>waste heat 40°</t>
-  </si>
-  <si>
     <t>various</t>
   </si>
   <si>
-    <t>gas. Biomass</t>
-  </si>
-  <si>
-    <t>gas/oil</t>
-  </si>
-  <si>
     <t>type</t>
   </si>
   <si>
@@ -283,18 +269,6 @@
     <t>heat pump</t>
   </si>
   <si>
-    <t>heat pump - High Temperature -Geo Thermal (60°C)</t>
-  </si>
-  <si>
-    <t>heat pump - Default</t>
-  </si>
-  <si>
-    <t>heat pump - River 5°C</t>
-  </si>
-  <si>
-    <t>heat pump - River 10°C</t>
-  </si>
-  <si>
     <t>Power To Heat</t>
   </si>
   <si>
@@ -388,17 +362,113 @@
     <t>Technologies</t>
   </si>
   <si>
-    <t>Solar Thermal Default</t>
-  </si>
-  <si>
-    <t>heat pump default</t>
+    <t>CHP-SE#Default</t>
+  </si>
+  <si>
+    <t>Pmax</t>
+  </si>
+  <si>
+    <t>heat pump # Heat Pump (River 10°C)</t>
+  </si>
+  <si>
+    <t>heat pump # Heat Pump (River 5°C)</t>
+  </si>
+  <si>
+    <t>Heat Pump (River 10°C)</t>
+  </si>
+  <si>
+    <t>Heat Pump (River 5°C)</t>
+  </si>
+  <si>
+    <t>Heat Pump (Geothermal 60°C)</t>
+  </si>
+  <si>
+    <t>Heat Pump (Geothermal 80°C)</t>
+  </si>
+  <si>
+    <t>heat pump # Heat Pump (Geothermal 80°C)</t>
+  </si>
+  <si>
+    <t>heat pump # Heat Pump (Geothermal 60°C)</t>
+  </si>
+  <si>
+    <t>Gas turbine</t>
+  </si>
+  <si>
+    <t>oil</t>
+  </si>
+  <si>
+    <t>hard coal</t>
+  </si>
+  <si>
+    <t>biogas</t>
+  </si>
+  <si>
+    <t>various 1</t>
+  </si>
+  <si>
+    <t>various 2</t>
+  </si>
+  <si>
+    <t>various 3</t>
+  </si>
+  <si>
+    <t>various 4</t>
+  </si>
+  <si>
+    <t>biomass</t>
+  </si>
+  <si>
+    <t xml:space="preserve">straw </t>
+  </si>
+  <si>
+    <t>Default Waste Inceneration Plant</t>
+  </si>
+  <si>
+    <t>Geothermal Plant</t>
+  </si>
+  <si>
+    <t>Default Power to Heat Plant</t>
+  </si>
+  <si>
+    <t>CHP-SE steam turbine (medium) wood chips</t>
+  </si>
+  <si>
+    <t>CHP-SE steam turbine (small) wood chips</t>
+  </si>
+  <si>
+    <t>CHP-SE steam turbine (medium) straw</t>
+  </si>
+  <si>
+    <t>CHP-SE steam turbine (small) straw</t>
+  </si>
+  <si>
+    <t>CHP-SE waste treatment waste</t>
+  </si>
+  <si>
+    <t>Excess Heat Plant</t>
+  </si>
+  <si>
+    <t>CHP-BP stirling engine gas. Biomass</t>
+  </si>
+  <si>
+    <t>CHP-BP spark ignition natural gas</t>
+  </si>
+  <si>
+    <t>CHP-BP spark ignition gas. Biomass</t>
+  </si>
+  <si>
+    <t>Default Solar Thermal</t>
+  </si>
+  <si>
+    <t>various 5</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -440,6 +510,13 @@
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="6">
@@ -527,23 +604,14 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -559,9 +627,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -587,6 +652,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -594,7 +669,66 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Eingabe" xfId="3" builtinId="20"/>
@@ -936,10 +1070,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N23"/>
+  <dimension ref="A1:N29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -961,85 +1095,85 @@
     <col min="16" max="16" width="48.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="18" t="s">
+    <row r="1" spans="1:14" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="D1" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="E1" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="F1" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="G1" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="H1" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="I1" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="J1" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="K1" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="L1" s="15" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="G2" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="H2" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="C1" s="18" t="s">
-        <v>36</v>
-      </c>
-      <c r="D1" s="18" t="s">
-        <v>32</v>
-      </c>
-      <c r="E1" s="18" t="s">
-        <v>39</v>
-      </c>
-      <c r="F1" s="18" t="s">
-        <v>38</v>
-      </c>
-      <c r="G1" s="18" t="s">
-        <v>28</v>
-      </c>
-      <c r="H1" s="18" t="s">
-        <v>30</v>
-      </c>
-      <c r="I1" s="18" t="s">
-        <v>31</v>
-      </c>
-      <c r="J1" s="18" t="s">
-        <v>29</v>
-      </c>
-      <c r="K1" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="L1" s="19" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" s="10" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="18" t="s">
-        <v>18</v>
-      </c>
-      <c r="B2" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="C2" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="D2" s="18" t="s">
+      <c r="I2" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="E2" s="18" t="s">
+      <c r="J2" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="F2" s="18" t="s">
+      <c r="K2" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="G2" s="18" t="s">
-        <v>22</v>
-      </c>
-      <c r="H2" s="18" t="s">
-        <v>23</v>
-      </c>
-      <c r="I2" s="18" t="s">
-        <v>24</v>
-      </c>
-      <c r="J2" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="K2" s="18" t="s">
-        <v>26</v>
-      </c>
-      <c r="L2" s="20" t="s">
-        <v>68</v>
+      <c r="L2" s="16" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="21" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
       <c r="B3" s="21" t="s">
         <v>0</v>
@@ -1051,19 +1185,19 @@
         <v>0</v>
       </c>
       <c r="E3" s="21">
-        <v>1.03</v>
+        <v>0.9</v>
       </c>
       <c r="F3" s="21">
         <v>0</v>
       </c>
       <c r="G3" s="21">
-        <v>60000</v>
+        <v>100000</v>
       </c>
       <c r="H3" s="21">
-        <v>2000</v>
+        <v>4000</v>
       </c>
       <c r="I3" s="21">
-        <v>1.1000000000000001</v>
+        <v>0.5</v>
       </c>
       <c r="J3" s="21">
         <v>25</v>
@@ -1078,7 +1212,7 @@
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="21" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="B4" s="21" t="s">
         <v>0</v>
@@ -1096,13 +1230,13 @@
         <v>0</v>
       </c>
       <c r="G4" s="21">
-        <v>800000</v>
+        <v>670000</v>
       </c>
       <c r="H4" s="22">
-        <v>0</v>
+        <v>13000</v>
       </c>
       <c r="I4" s="21">
-        <v>5.4</v>
+        <v>2.9</v>
       </c>
       <c r="J4" s="21">
         <v>20</v>
@@ -1117,7 +1251,7 @@
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="21" t="s">
-        <v>103</v>
+        <v>94</v>
       </c>
       <c r="B5" s="21" t="s">
         <v>0</v>
@@ -1135,13 +1269,13 @@
         <v>0</v>
       </c>
       <c r="G5" s="21">
-        <v>400000</v>
+        <v>700000</v>
       </c>
       <c r="H5" s="22">
-        <v>0</v>
+        <v>13000</v>
       </c>
       <c r="I5" s="21">
-        <v>2.7</v>
+        <v>3</v>
       </c>
       <c r="J5" s="22">
         <v>20</v>
@@ -1156,7 +1290,7 @@
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="21" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
       <c r="B6" s="21" t="s">
         <v>0</v>
@@ -1168,19 +1302,19 @@
         <v>0</v>
       </c>
       <c r="E6" s="22">
-        <v>0.85</v>
+        <v>0.83</v>
       </c>
       <c r="F6" s="21">
         <v>0</v>
       </c>
       <c r="G6" s="21">
-        <v>800000</v>
+        <v>750000</v>
       </c>
       <c r="H6" s="22">
-        <v>0</v>
+        <v>13000</v>
       </c>
       <c r="I6" s="21">
-        <v>4</v>
+        <v>3.1</v>
       </c>
       <c r="J6" s="22">
         <v>20</v>
@@ -1195,7 +1329,7 @@
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="21" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="B7" s="21" t="s">
         <v>0</v>
@@ -1207,7 +1341,7 @@
         <v>0</v>
       </c>
       <c r="E7" s="21">
-        <v>0.98</v>
+        <v>0.81</v>
       </c>
       <c r="F7" s="21">
         <v>0</v>
@@ -1216,16 +1350,16 @@
         <v>1200000</v>
       </c>
       <c r="H7" s="21">
-        <v>54000</v>
+        <v>230000</v>
       </c>
       <c r="I7" s="21">
-        <v>5.6</v>
+        <v>0.5</v>
       </c>
       <c r="J7" s="21">
         <v>20</v>
       </c>
       <c r="K7" s="22">
-        <v>0.3</v>
+        <v>0.5</v>
       </c>
       <c r="L7" s="21">
         <v>0</v>
@@ -1234,7 +1368,7 @@
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="21" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="B8" s="21" t="s">
         <v>0</v>
@@ -1255,10 +1389,10 @@
         <v>150000</v>
       </c>
       <c r="H8" s="21">
-        <v>1100</v>
+        <v>2000</v>
       </c>
       <c r="I8" s="21">
-        <v>0.8</v>
+        <v>0.5</v>
       </c>
       <c r="J8" s="21">
         <v>20</v>
@@ -1273,13 +1407,13 @@
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="21" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="B9" s="21" t="s">
         <v>0</v>
       </c>
       <c r="C9" s="21" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D9" s="21">
         <v>0</v>
@@ -1291,19 +1425,19 @@
         <v>0</v>
       </c>
       <c r="G9" s="21">
-        <v>0</v>
+        <v>1600000</v>
       </c>
       <c r="H9" s="21">
-        <v>0</v>
+        <v>35000</v>
       </c>
       <c r="I9" s="21">
         <v>0</v>
       </c>
       <c r="J9" s="21">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="K9" s="22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L9" s="21">
         <v>0</v>
@@ -1318,31 +1452,31 @@
         <v>83</v>
       </c>
       <c r="C10" s="21" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="D10" s="21">
         <v>0</v>
       </c>
       <c r="E10" s="22">
-        <v>4</v>
+        <v>0.46</v>
       </c>
       <c r="F10" s="21">
-        <v>0</v>
+        <v>0.37</v>
       </c>
       <c r="G10" s="21">
-        <v>700000</v>
+        <v>875000</v>
       </c>
       <c r="H10" s="21">
-        <v>2000</v>
+        <v>23000</v>
       </c>
       <c r="I10" s="21">
-        <v>8.4</v>
+        <v>1.7</v>
       </c>
       <c r="J10" s="21">
         <v>25</v>
       </c>
       <c r="K10" s="22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L10" s="21">
         <v>0</v>
@@ -1354,10 +1488,10 @@
         <v>2</v>
       </c>
       <c r="B11" s="21" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="C11" s="21" t="s">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="D11" s="21">
         <v>0</v>
@@ -1366,16 +1500,16 @@
         <v>0.35</v>
       </c>
       <c r="F11" s="21">
-        <v>0.55000000000000004</v>
+        <v>0.5</v>
       </c>
       <c r="G11" s="21">
-        <v>900000</v>
+        <v>1500000</v>
       </c>
       <c r="H11" s="21">
-        <v>30000</v>
+        <v>34000</v>
       </c>
       <c r="I11" s="21">
-        <v>4.5</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="J11" s="21">
         <v>25</v>
@@ -1393,25 +1527,25 @@
         <v>3</v>
       </c>
       <c r="B12" s="23" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="C12" s="21" t="s">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="D12" s="21">
         <v>0</v>
       </c>
       <c r="E12" s="22">
-        <v>0.45</v>
+        <v>0.36</v>
       </c>
       <c r="F12" s="21">
-        <v>0.47</v>
+        <v>0.5</v>
       </c>
       <c r="G12" s="21">
         <v>1300000</v>
       </c>
       <c r="H12" s="21">
-        <v>30000</v>
+        <v>34000</v>
       </c>
       <c r="I12" s="21">
         <v>4.5</v>
@@ -1425,17 +1559,16 @@
       <c r="L12" s="21">
         <v>0</v>
       </c>
-      <c r="N12"/>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="24" t="s">
-        <v>119</v>
+        <v>142</v>
       </c>
       <c r="B13" s="24" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="C13" s="24" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="D13" s="24">
         <v>0</v>
@@ -1453,7 +1586,7 @@
         <v>10000</v>
       </c>
       <c r="I13" s="24">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="J13" s="24">
         <v>20</v>
@@ -1464,37 +1597,618 @@
       <c r="L13" s="25">
         <v>0</v>
       </c>
-      <c r="N13"/>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="N14"/>
+      <c r="A14" s="17" t="s">
+        <v>117</v>
+      </c>
+      <c r="B14" s="17" t="s">
+        <v>78</v>
+      </c>
+      <c r="C14" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="D14" s="17">
+        <v>0</v>
+      </c>
+      <c r="E14" s="18">
+        <v>4</v>
+      </c>
+      <c r="F14" s="33">
+        <v>0</v>
+      </c>
+      <c r="G14" s="33">
+        <v>510000</v>
+      </c>
+      <c r="H14" s="33">
+        <v>10000</v>
+      </c>
+      <c r="I14" s="33">
+        <v>0.5</v>
+      </c>
+      <c r="J14" s="33">
+        <v>25</v>
+      </c>
+      <c r="K14" s="34">
+        <v>0.75</v>
+      </c>
+      <c r="L14" s="33">
+        <v>0</v>
+      </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A15" s="17" t="s">
+        <v>116</v>
+      </c>
+      <c r="B15" s="17" t="s">
+        <v>78</v>
+      </c>
+      <c r="C15" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="D15" s="17">
+        <v>0</v>
+      </c>
+      <c r="E15" s="18">
+        <v>4</v>
+      </c>
+      <c r="F15" s="35">
+        <v>0</v>
+      </c>
+      <c r="G15" s="35">
+        <v>510000</v>
+      </c>
+      <c r="H15" s="35">
+        <v>10000</v>
+      </c>
+      <c r="I15" s="35">
+        <v>0.5</v>
+      </c>
+      <c r="J15" s="35">
+        <v>25</v>
+      </c>
+      <c r="K15" s="36">
+        <v>0.75</v>
+      </c>
+      <c r="L15" s="35">
+        <v>0</v>
+      </c>
       <c r="N15"/>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A16" s="17" t="s">
+        <v>114</v>
+      </c>
+      <c r="B16" s="17" t="s">
+        <v>78</v>
+      </c>
+      <c r="C16" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="D16" s="17">
+        <v>0</v>
+      </c>
+      <c r="E16" s="18">
+        <v>4</v>
+      </c>
+      <c r="F16" s="37">
+        <v>0</v>
+      </c>
+      <c r="G16" s="37">
+        <v>510000</v>
+      </c>
+      <c r="H16" s="37">
+        <v>10000</v>
+      </c>
+      <c r="I16" s="37">
+        <v>0.5</v>
+      </c>
+      <c r="J16" s="37">
+        <v>25</v>
+      </c>
+      <c r="K16" s="38">
+        <v>0.75</v>
+      </c>
+      <c r="L16" s="37">
+        <v>0</v>
+      </c>
       <c r="N16"/>
     </row>
-    <row r="17" spans="14:14" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="17" t="s">
+        <v>115</v>
+      </c>
+      <c r="B17" s="17" t="s">
+        <v>78</v>
+      </c>
+      <c r="C17" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="D17" s="17">
+        <v>0</v>
+      </c>
+      <c r="E17" s="18">
+        <v>4</v>
+      </c>
+      <c r="F17" s="40">
+        <v>0</v>
+      </c>
+      <c r="G17" s="40">
+        <v>510000</v>
+      </c>
+      <c r="H17" s="40">
+        <v>10000</v>
+      </c>
+      <c r="I17" s="40">
+        <v>0.5</v>
+      </c>
+      <c r="J17" s="40">
+        <v>25</v>
+      </c>
+      <c r="K17" s="41">
+        <v>0.75</v>
+      </c>
+      <c r="L17" s="40">
+        <v>0</v>
+      </c>
       <c r="N17"/>
     </row>
-    <row r="18" spans="14:14" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A18" s="45" t="s">
+        <v>130</v>
+      </c>
+      <c r="B18" s="45" t="s">
+        <v>1</v>
+      </c>
+      <c r="C18" s="45" t="s">
+        <v>8</v>
+      </c>
+      <c r="D18" s="45">
+        <v>0</v>
+      </c>
+      <c r="E18" s="45">
+        <v>0.75</v>
+      </c>
+      <c r="F18" s="45">
+        <v>0.3</v>
+      </c>
+      <c r="G18" s="45">
+        <v>1200000</v>
+      </c>
+      <c r="H18" s="45">
+        <v>54000</v>
+      </c>
+      <c r="I18" s="45">
+        <v>5.6</v>
+      </c>
+      <c r="J18" s="45">
+        <v>20</v>
+      </c>
+      <c r="K18" s="45">
+        <v>0</v>
+      </c>
+      <c r="L18" s="45">
+        <v>0</v>
+      </c>
       <c r="N18"/>
     </row>
-    <row r="19" spans="14:14" x14ac:dyDescent="0.25">
-      <c r="N19"/>
-    </row>
-    <row r="20" spans="14:14" x14ac:dyDescent="0.25">
-      <c r="N20"/>
-    </row>
-    <row r="21" spans="14:14" x14ac:dyDescent="0.25">
-      <c r="N21"/>
-    </row>
-    <row r="22" spans="14:14" x14ac:dyDescent="0.25">
-      <c r="N22"/>
-    </row>
-    <row r="23" spans="14:14" x14ac:dyDescent="0.25">
-      <c r="N23"/>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A19" s="45" t="s">
+        <v>132</v>
+      </c>
+      <c r="B19" s="45" t="s">
+        <v>79</v>
+      </c>
+      <c r="C19" s="45" t="s">
+        <v>9</v>
+      </c>
+      <c r="D19" s="45">
+        <v>0</v>
+      </c>
+      <c r="E19" s="45">
+        <v>0</v>
+      </c>
+      <c r="F19" s="45">
+        <v>0</v>
+      </c>
+      <c r="G19" s="45">
+        <v>0</v>
+      </c>
+      <c r="H19" s="45">
+        <v>0</v>
+      </c>
+      <c r="I19" s="45">
+        <v>0</v>
+      </c>
+      <c r="J19" s="45">
+        <v>0</v>
+      </c>
+      <c r="K19" s="45">
+        <v>0</v>
+      </c>
+      <c r="L19" s="45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A20" s="45" t="s">
+        <v>138</v>
+      </c>
+      <c r="B20" s="45" t="s">
+        <v>80</v>
+      </c>
+      <c r="C20" s="45" t="s">
+        <v>124</v>
+      </c>
+      <c r="D20" s="45">
+        <v>0</v>
+      </c>
+      <c r="E20" s="45">
+        <v>0</v>
+      </c>
+      <c r="F20" s="45">
+        <v>0</v>
+      </c>
+      <c r="G20" s="45">
+        <v>0</v>
+      </c>
+      <c r="H20" s="45">
+        <v>0</v>
+      </c>
+      <c r="I20" s="45">
+        <v>0</v>
+      </c>
+      <c r="J20" s="45">
+        <v>0</v>
+      </c>
+      <c r="K20" s="45">
+        <v>0</v>
+      </c>
+      <c r="L20" s="45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A21" s="45" t="s">
+        <v>131</v>
+      </c>
+      <c r="B21" s="45" t="s">
+        <v>81</v>
+      </c>
+      <c r="C21" s="45" t="s">
+        <v>125</v>
+      </c>
+      <c r="D21" s="45">
+        <v>0</v>
+      </c>
+      <c r="E21" s="45">
+        <v>0.1</v>
+      </c>
+      <c r="F21" s="45">
+        <v>0</v>
+      </c>
+      <c r="G21" s="45">
+        <v>0</v>
+      </c>
+      <c r="H21" s="45">
+        <v>0</v>
+      </c>
+      <c r="I21" s="45">
+        <v>0</v>
+      </c>
+      <c r="J21" s="45">
+        <v>0</v>
+      </c>
+      <c r="K21" s="45">
+        <v>0</v>
+      </c>
+      <c r="L21" s="45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A22" s="45" t="s">
+        <v>133</v>
+      </c>
+      <c r="B22" s="45" t="s">
+        <v>83</v>
+      </c>
+      <c r="C22" s="45" t="s">
+        <v>5</v>
+      </c>
+      <c r="D22" s="45">
+        <v>0</v>
+      </c>
+      <c r="E22" s="45">
+        <v>0.64</v>
+      </c>
+      <c r="F22" s="45">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="G22" s="45">
+        <v>4000000</v>
+      </c>
+      <c r="H22" s="45">
+        <v>29000</v>
+      </c>
+      <c r="I22" s="45">
+        <v>3.9</v>
+      </c>
+      <c r="J22" s="45">
+        <v>30</v>
+      </c>
+      <c r="K22" s="45">
+        <v>1</v>
+      </c>
+      <c r="L22" s="45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A23" s="45" t="s">
+        <v>134</v>
+      </c>
+      <c r="B23" s="45" t="s">
+        <v>83</v>
+      </c>
+      <c r="C23" s="45" t="s">
+        <v>5</v>
+      </c>
+      <c r="D23" s="45">
+        <v>0</v>
+      </c>
+      <c r="E23" s="45">
+        <v>0.62</v>
+      </c>
+      <c r="F23" s="45">
+        <v>0.25</v>
+      </c>
+      <c r="G23" s="45">
+        <v>6000000</v>
+      </c>
+      <c r="H23" s="45">
+        <v>150000</v>
+      </c>
+      <c r="I23" s="45">
+        <v>0</v>
+      </c>
+      <c r="J23" s="45">
+        <v>20</v>
+      </c>
+      <c r="K23" s="45">
+        <v>1</v>
+      </c>
+      <c r="L23" s="45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A24" s="45" t="s">
+        <v>135</v>
+      </c>
+      <c r="B24" s="45" t="s">
+        <v>83</v>
+      </c>
+      <c r="C24" s="45" t="s">
+        <v>7</v>
+      </c>
+      <c r="D24" s="45">
+        <v>0</v>
+      </c>
+      <c r="E24" s="45">
+        <v>0.64</v>
+      </c>
+      <c r="F24" s="45">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="G24" s="45">
+        <v>4000000</v>
+      </c>
+      <c r="H24" s="45">
+        <v>40000</v>
+      </c>
+      <c r="I24" s="45">
+        <v>6.4</v>
+      </c>
+      <c r="J24" s="45">
+        <v>25</v>
+      </c>
+      <c r="K24" s="45">
+        <v>1</v>
+      </c>
+      <c r="L24" s="45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A25" s="45" t="s">
+        <v>136</v>
+      </c>
+      <c r="B25" s="45" t="s">
+        <v>83</v>
+      </c>
+      <c r="C25" s="45" t="s">
+        <v>7</v>
+      </c>
+      <c r="D25" s="45">
+        <v>0</v>
+      </c>
+      <c r="E25" s="45">
+        <v>0.62</v>
+      </c>
+      <c r="F25" s="45">
+        <v>0.3</v>
+      </c>
+      <c r="G25" s="45">
+        <v>6000000</v>
+      </c>
+      <c r="H25" s="45">
+        <v>150000</v>
+      </c>
+      <c r="I25" s="45">
+        <v>0</v>
+      </c>
+      <c r="J25" s="45">
+        <v>20</v>
+      </c>
+      <c r="K25" s="45">
+        <v>1</v>
+      </c>
+      <c r="L25" s="45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A26" s="45" t="s">
+        <v>137</v>
+      </c>
+      <c r="B26" s="45" t="s">
+        <v>83</v>
+      </c>
+      <c r="C26" s="45" t="s">
+        <v>8</v>
+      </c>
+      <c r="D26" s="45">
+        <v>0</v>
+      </c>
+      <c r="E26" s="45">
+        <v>0.62</v>
+      </c>
+      <c r="F26" s="45">
+        <v>0.24</v>
+      </c>
+      <c r="G26" s="45">
+        <v>8500000</v>
+      </c>
+      <c r="H26" s="45">
+        <v>150000</v>
+      </c>
+      <c r="I26" s="45">
+        <v>0</v>
+      </c>
+      <c r="J26" s="45">
+        <v>20</v>
+      </c>
+      <c r="K26" s="45">
+        <v>1</v>
+      </c>
+      <c r="L26" s="45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A27" s="45" t="s">
+        <v>139</v>
+      </c>
+      <c r="B27" s="45" t="s">
+        <v>82</v>
+      </c>
+      <c r="C27" s="45" t="s">
+        <v>123</v>
+      </c>
+      <c r="D27" s="45">
+        <v>0</v>
+      </c>
+      <c r="E27" s="45">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="F27" s="45">
+        <v>0.2</v>
+      </c>
+      <c r="G27" s="45">
+        <v>5000000</v>
+      </c>
+      <c r="H27" s="45">
+        <v>32000</v>
+      </c>
+      <c r="I27" s="45">
+        <v>26</v>
+      </c>
+      <c r="J27" s="45">
+        <v>15</v>
+      </c>
+      <c r="K27" s="45">
+        <v>1</v>
+      </c>
+      <c r="L27" s="45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A28" s="45" t="s">
+        <v>140</v>
+      </c>
+      <c r="B28" s="45" t="s">
+        <v>82</v>
+      </c>
+      <c r="C28" s="45" t="s">
+        <v>4</v>
+      </c>
+      <c r="D28" s="45">
+        <v>0</v>
+      </c>
+      <c r="E28" s="45">
+        <v>0.45</v>
+      </c>
+      <c r="F28" s="45">
+        <v>0.44</v>
+      </c>
+      <c r="G28" s="45">
+        <v>1000000</v>
+      </c>
+      <c r="H28" s="45">
+        <v>10000</v>
+      </c>
+      <c r="I28" s="45">
+        <v>5.4</v>
+      </c>
+      <c r="J28" s="45">
+        <v>25</v>
+      </c>
+      <c r="K28" s="45">
+        <v>1</v>
+      </c>
+      <c r="L28" s="45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A29" s="45" t="s">
+        <v>141</v>
+      </c>
+      <c r="B29" s="45" t="s">
+        <v>82</v>
+      </c>
+      <c r="C29" s="45" t="s">
+        <v>123</v>
+      </c>
+      <c r="D29" s="45">
+        <v>0</v>
+      </c>
+      <c r="E29" s="45">
+        <v>0.45</v>
+      </c>
+      <c r="F29" s="45">
+        <v>0.4</v>
+      </c>
+      <c r="G29" s="45">
+        <v>1000000</v>
+      </c>
+      <c r="H29" s="45">
+        <v>10000</v>
+      </c>
+      <c r="I29" s="45">
+        <v>8</v>
+      </c>
+      <c r="J29" s="45">
+        <v>25</v>
+      </c>
+      <c r="K29" s="45">
+        <v>1</v>
+      </c>
+      <c r="L29" s="45">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1502,183 +2216,252 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8DB2E28E-E92F-43F4-9695-A47154FC866C}">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H24" sqref="H24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.140625" customWidth="1"/>
     <col min="2" max="2" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="11" t="s">
+    <row r="1" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="26" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="31" t="s">
+        <v>35</v>
+      </c>
+      <c r="C3" s="29">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="26" t="s">
+        <v>123</v>
+      </c>
+      <c r="B4" s="28">
+        <v>100</v>
+      </c>
+      <c r="C4" s="29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="26" t="s">
+        <v>121</v>
+      </c>
+      <c r="B5" s="28">
+        <v>55.4</v>
+      </c>
+      <c r="C5" s="29">
+        <v>0.28000000000000003</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="26" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="30">
+        <v>29.8</v>
+      </c>
+      <c r="C6" s="29">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="26" t="s">
+        <v>122</v>
+      </c>
+      <c r="B7" s="28">
+        <v>7.7</v>
+      </c>
+      <c r="C7" s="29">
+        <v>0.34</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="26" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="28">
+        <v>1</v>
+      </c>
+      <c r="C8" s="29">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9" s="2">
+        <v>22</v>
+      </c>
+      <c r="C9" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" s="2">
         <v>36</v>
       </c>
-      <c r="B1" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="C1" s="11" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="B2" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="C2" s="11" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" s="5">
-        <v>0</v>
-      </c>
-      <c r="C3" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="C4" s="2">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="B5" s="5">
+      <c r="C10" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="44" t="s">
+        <v>128</v>
+      </c>
+      <c r="B11" s="44">
         <v>62</v>
       </c>
-      <c r="C5" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B6" s="5">
-        <v>47</v>
-      </c>
-      <c r="C6" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B7" s="6">
-        <v>30</v>
-      </c>
-      <c r="C7" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8" s="5">
+      <c r="C11" s="44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="44" t="s">
+        <v>129</v>
+      </c>
+      <c r="B12" s="44">
         <v>22</v>
       </c>
-      <c r="C8" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B9" s="5">
-        <v>20</v>
-      </c>
-      <c r="C9" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B10" s="5">
-        <v>5</v>
-      </c>
-      <c r="C10" s="2">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B11" s="5">
-        <v>0</v>
-      </c>
-      <c r="C11" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B12" s="5">
-        <v>0</v>
-      </c>
-      <c r="C12" s="2">
-        <v>1</v>
+      <c r="C12" s="44">
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B13" s="5">
-        <v>22</v>
-      </c>
-      <c r="C13" s="2">
-        <v>1</v>
+      <c r="A13" s="27" t="s">
+        <v>38</v>
+      </c>
+      <c r="B13" s="28">
+        <v>0</v>
+      </c>
+      <c r="C13" s="29">
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B14" s="5">
-        <v>36</v>
-      </c>
-      <c r="C14" s="2">
-        <v>1</v>
+      <c r="A14" s="39" t="s">
+        <v>124</v>
+      </c>
+      <c r="B14" s="28">
+        <v>0</v>
+      </c>
+      <c r="C14" s="29">
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="13" t="s">
-        <v>43</v>
-      </c>
-      <c r="B15" s="5">
-        <v>0</v>
-      </c>
-      <c r="C15" s="2">
+      <c r="A15" s="39" t="s">
+        <v>125</v>
+      </c>
+      <c r="B15" s="28">
+        <v>0</v>
+      </c>
+      <c r="C15" s="29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="39" t="s">
+        <v>126</v>
+      </c>
+      <c r="B16" s="42">
+        <v>0</v>
+      </c>
+      <c r="C16" s="43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="39" t="s">
+        <v>127</v>
+      </c>
+      <c r="B17" s="42">
+        <v>0</v>
+      </c>
+      <c r="C17" s="43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="39" t="s">
+        <v>143</v>
+      </c>
+      <c r="B18" s="42">
+        <v>0</v>
+      </c>
+      <c r="C18" s="43">
         <v>0</v>
       </c>
     </row>
@@ -1705,44 +2488,44 @@
     <col min="6" max="6" width="20.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
+    <row r="1" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="E1" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="F1" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="C1" s="9" t="s">
+    </row>
+    <row r="2" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="F2" s="6" t="s">
         <v>44</v>
-      </c>
-      <c r="D1" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="E1" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="F1" s="9" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="9" t="s">
-        <v>95</v>
-      </c>
-      <c r="B2" s="9" t="s">
-        <v>69</v>
-      </c>
-      <c r="C2" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="D2" s="9" t="s">
-        <v>93</v>
-      </c>
-      <c r="E2" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="F2" s="9" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -1761,7 +2544,7 @@
       <c r="E3" s="2">
         <v>1</v>
       </c>
-      <c r="F3" s="7">
+      <c r="F3" s="4">
         <v>6000000</v>
       </c>
     </row>
@@ -1775,7 +2558,7 @@
   <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1793,98 +2576,98 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="G1" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="H1" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="I1" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="J1" s="8" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="C2" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="E2" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="C1" s="11" t="s">
-        <v>97</v>
-      </c>
-      <c r="D1" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="E1" s="11" t="s">
-        <v>54</v>
-      </c>
-      <c r="F1" s="11" t="s">
+      <c r="F2" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="G1" s="11" t="s">
+      <c r="G2" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="H1" s="11" t="s">
-        <v>58</v>
-      </c>
-      <c r="I1" s="11" t="s">
+      <c r="H2" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="I2" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="J2" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="J1" s="11" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="B2" s="11" t="s">
-        <v>56</v>
-      </c>
-      <c r="C2" s="11" t="s">
-        <v>98</v>
-      </c>
-      <c r="D2" s="14" t="s">
-        <v>63</v>
-      </c>
-      <c r="E2" s="11" t="s">
-        <v>64</v>
-      </c>
-      <c r="F2" s="11" t="s">
-        <v>65</v>
-      </c>
-      <c r="G2" s="11" t="s">
-        <v>66</v>
-      </c>
-      <c r="H2" s="11" t="s">
-        <v>96</v>
-      </c>
-      <c r="I2" s="11" t="s">
-        <v>99</v>
-      </c>
-      <c r="J2" s="11" t="s">
-        <v>57</v>
-      </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="B3" s="3">
+        <v>0</v>
+      </c>
+      <c r="C3" s="3">
+        <v>1</v>
+      </c>
+      <c r="D3" s="3">
+        <v>0</v>
+      </c>
+      <c r="E3" s="3">
+        <v>0</v>
+      </c>
+      <c r="F3" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="G3" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="H3" s="32">
+        <v>5000</v>
+      </c>
+      <c r="I3" s="32">
         <v>100</v>
       </c>
-      <c r="B3" s="4">
-        <v>0</v>
-      </c>
-      <c r="C3" s="4">
-        <v>1</v>
-      </c>
-      <c r="D3" s="4">
-        <v>80</v>
-      </c>
-      <c r="E3" s="4">
-        <v>80</v>
-      </c>
-      <c r="F3" s="4">
-        <v>0.95</v>
-      </c>
-      <c r="G3" s="4">
-        <v>0.95</v>
-      </c>
-      <c r="H3" s="4">
-        <v>60</v>
-      </c>
-      <c r="I3" s="4">
-        <v>10000</v>
-      </c>
-      <c r="J3" s="4">
+      <c r="J3" s="3">
         <v>25</v>
       </c>
     </row>
@@ -1899,7 +2682,7 @@
   <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="A6" sqref="A6:A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1909,83 +2692,83 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="19" t="s">
-        <v>118</v>
-      </c>
-      <c r="B1" s="26" t="s">
-        <v>108</v>
+      <c r="A1" s="15" t="s">
+        <v>109</v>
+      </c>
+      <c r="B1" s="19" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="15" t="s">
+      <c r="A2" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="B2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="11" t="s">
         <v>83</v>
       </c>
-      <c r="B2" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="15" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="15" t="s">
-        <v>92</v>
-      </c>
       <c r="B4" t="s">
-        <v>111</v>
+        <v>102</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="B5" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="15" t="s">
+      <c r="A6" s="11" t="s">
         <v>1</v>
       </c>
       <c r="B6" t="s">
-        <v>113</v>
+        <v>104</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="15" t="s">
-        <v>62</v>
+      <c r="A7" s="11" t="s">
+        <v>57</v>
       </c>
       <c r="B7" t="s">
-        <v>114</v>
+        <v>105</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="15" t="s">
-        <v>88</v>
+      <c r="A8" s="11" t="s">
+        <v>79</v>
       </c>
       <c r="B8" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="15" t="s">
-        <v>89</v>
+      <c r="A9" s="11" t="s">
+        <v>80</v>
       </c>
       <c r="B9" t="s">
-        <v>116</v>
+        <v>107</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="15" t="s">
-        <v>90</v>
+      <c r="A10" s="11" t="s">
+        <v>81</v>
       </c>
       <c r="B10" t="s">
-        <v>117</v>
+        <v>108</v>
       </c>
     </row>
   </sheetData>
@@ -2004,35 +2787,35 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>84</v>
+        <v>118</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="17" t="s">
+      <c r="A2" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="B2" t="s">
+        <v>66</v>
+      </c>
+      <c r="C2" t="s">
+        <v>67</v>
+      </c>
+      <c r="D2" t="s">
+        <v>68</v>
+      </c>
+      <c r="E2" t="s">
+        <v>69</v>
+      </c>
+      <c r="F2" t="s">
         <v>70</v>
       </c>
-      <c r="B2" t="s">
+      <c r="G2" t="s">
         <v>71</v>
-      </c>
-      <c r="C2" t="s">
-        <v>72</v>
-      </c>
-      <c r="D2" t="s">
-        <v>73</v>
-      </c>
-      <c r="E2" t="s">
-        <v>74</v>
-      </c>
-      <c r="F2" t="s">
-        <v>75</v>
-      </c>
-      <c r="G2" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="B3">
         <v>48.67</v>
@@ -2055,7 +2838,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="B4">
         <v>40.96</v>
@@ -2078,7 +2861,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="B5">
         <v>23.95</v>
@@ -2101,7 +2884,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -2124,7 +2907,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="B7">
         <v>0</v>
@@ -2147,7 +2930,7 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="B8">
         <v>0</v>
@@ -2170,7 +2953,7 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="B9">
         <v>0</v>
@@ -2206,35 +2989,35 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>85</v>
+        <v>119</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="16" t="s">
+      <c r="A2" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="B2" t="s">
+        <v>66</v>
+      </c>
+      <c r="C2" t="s">
+        <v>67</v>
+      </c>
+      <c r="D2" t="s">
+        <v>68</v>
+      </c>
+      <c r="E2" t="s">
+        <v>69</v>
+      </c>
+      <c r="F2" t="s">
         <v>70</v>
       </c>
-      <c r="B2" t="s">
+      <c r="G2" t="s">
         <v>71</v>
       </c>
-      <c r="C2" t="s">
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="12" t="s">
         <v>72</v>
-      </c>
-      <c r="D2" t="s">
-        <v>73</v>
-      </c>
-      <c r="E2" t="s">
-        <v>74</v>
-      </c>
-      <c r="F2" t="s">
-        <v>75</v>
-      </c>
-      <c r="G2" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="16" t="s">
-        <v>77</v>
       </c>
       <c r="B3">
         <v>5.01</v>
@@ -2256,8 +3039,8 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="16" t="s">
-        <v>78</v>
+      <c r="A4" s="12" t="s">
+        <v>73</v>
       </c>
       <c r="B4">
         <v>4.76</v>
@@ -2279,8 +3062,8 @@
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="16" t="s">
-        <v>79</v>
+      <c r="A5" s="12" t="s">
+        <v>74</v>
       </c>
       <c r="B5">
         <v>4.6399999999999997</v>
@@ -2302,8 +3085,8 @@
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="16" t="s">
-        <v>80</v>
+      <c r="A6" s="12" t="s">
+        <v>75</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -2325,8 +3108,8 @@
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="16" t="s">
-        <v>81</v>
+      <c r="A7" s="12" t="s">
+        <v>76</v>
       </c>
       <c r="B7">
         <v>0</v>
@@ -2348,8 +3131,8 @@
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="16" t="s">
-        <v>82</v>
+      <c r="A8" s="12" t="s">
+        <v>77</v>
       </c>
       <c r="B8">
         <v>0</v>
@@ -2371,8 +3154,8 @@
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="16" t="s">
-        <v>71</v>
+      <c r="A9" s="12" t="s">
+        <v>66</v>
       </c>
       <c r="B9">
         <v>0</v>
@@ -2408,35 +3191,35 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>86</v>
+        <v>113</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B2" t="s">
+        <v>66</v>
+      </c>
+      <c r="C2" t="s">
+        <v>67</v>
+      </c>
+      <c r="D2" t="s">
+        <v>68</v>
+      </c>
+      <c r="E2" t="s">
+        <v>69</v>
+      </c>
+      <c r="F2" t="s">
         <v>70</v>
       </c>
-      <c r="B2" t="s">
+      <c r="G2" t="s">
         <v>71</v>
-      </c>
-      <c r="C2" t="s">
-        <v>72</v>
-      </c>
-      <c r="D2" t="s">
-        <v>73</v>
-      </c>
-      <c r="E2" t="s">
-        <v>74</v>
-      </c>
-      <c r="F2" t="s">
-        <v>75</v>
-      </c>
-      <c r="G2" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="B3">
         <v>3.08</v>
@@ -2459,7 +3242,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="B4">
         <v>2.99</v>
@@ -2482,7 +3265,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="B5">
         <v>2.94</v>
@@ -2505,7 +3288,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -2528,7 +3311,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="B7">
         <v>0</v>
@@ -2551,7 +3334,7 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="B8">
         <v>0</v>
@@ -2574,7 +3357,7 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="B9">
         <v>0</v>
@@ -2605,42 +3388,42 @@
   <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G32" sqref="G32"/>
+      <selection activeCell="J34" sqref="J34:J35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>87</v>
+        <v>112</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B2" t="s">
+        <v>66</v>
+      </c>
+      <c r="C2" t="s">
+        <v>67</v>
+      </c>
+      <c r="D2" t="s">
+        <v>68</v>
+      </c>
+      <c r="E2" t="s">
+        <v>69</v>
+      </c>
+      <c r="F2" t="s">
         <v>70</v>
       </c>
-      <c r="B2" t="s">
+      <c r="G2" t="s">
         <v>71</v>
-      </c>
-      <c r="C2" t="s">
-        <v>72</v>
-      </c>
-      <c r="D2" t="s">
-        <v>73</v>
-      </c>
-      <c r="E2" t="s">
-        <v>74</v>
-      </c>
-      <c r="F2" t="s">
-        <v>75</v>
-      </c>
-      <c r="G2" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="B3">
         <v>3.41</v>
@@ -2663,7 +3446,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="B4">
         <v>3.32</v>
@@ -2686,7 +3469,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="B5">
         <v>3.26</v>
@@ -2709,7 +3492,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -2732,7 +3515,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="B7">
         <v>0</v>
@@ -2755,7 +3538,7 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="B8">
         <v>0</v>
@@ -2778,7 +3561,7 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="B9">
         <v>0</v>

</xml_diff>

<commit_message>
add ramping costs for each technology , fix sum bugs
</commit_message>
<xml_diff>
--- a/app/modules/common/AD/F16_input/DH_technology_cost.xlsx
+++ b/app/modules/common/AD/F16_input/DH_technology_cost.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hasani\Documents\Workplace\Dispatch\app\modules\common\AD\F16_input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00E8E80D-F3FF-4709-9028-E2A328F32943}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20840857-490B-4C80-8878-38248B7BD61C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="10350" windowWidth="11970" windowHeight="4815" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -200,9 +200,6 @@
     <t>n_pump_hs</t>
   </si>
   <si>
-    <t>n_turb_hs</t>
-  </si>
-  <si>
     <t>Solar Thermal</t>
   </si>
   <si>
@@ -215,9 +212,6 @@
     <t>loading efficiency</t>
   </si>
   <si>
-    <t>unloading efficiency</t>
-  </si>
-  <si>
     <t>MR</t>
   </si>
   <si>
@@ -462,6 +456,12 @@
   </si>
   <si>
     <t>various 5</t>
+  </si>
+  <si>
+    <t>c_ramp</t>
+  </si>
+  <si>
+    <t>Ramping Costs [EUR/MWh]</t>
   </si>
 </sst>
 </file>
@@ -643,9 +643,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -728,6 +725,9 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1072,8 +1072,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B37" sqref="B37"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="K43" sqref="K43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1129,8 +1129,11 @@
       <c r="K1" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="L1" s="15" t="s">
-        <v>62</v>
+      <c r="L1" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="M1" s="39" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="2" spans="1:14" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -1167,1047 +1170,1131 @@
       <c r="K2" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="L2" s="16" t="s">
-        <v>63</v>
+      <c r="L2" s="45" t="s">
+        <v>61</v>
+      </c>
+      <c r="M2" s="39" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A3" s="21" t="s">
+      <c r="A3" s="20" t="s">
+        <v>90</v>
+      </c>
+      <c r="B3" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="20">
+        <v>0</v>
+      </c>
+      <c r="E3" s="20">
+        <v>0.9</v>
+      </c>
+      <c r="F3" s="20">
+        <v>0</v>
+      </c>
+      <c r="G3" s="20">
+        <v>100000</v>
+      </c>
+      <c r="H3" s="20">
+        <v>4000</v>
+      </c>
+      <c r="I3" s="20">
+        <v>0.5</v>
+      </c>
+      <c r="J3" s="20">
+        <v>25</v>
+      </c>
+      <c r="K3" s="21">
+        <v>0</v>
+      </c>
+      <c r="L3" s="20">
+        <v>0</v>
+      </c>
+      <c r="M3" s="39">
+        <v>0</v>
+      </c>
+      <c r="N3"/>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4" s="20" t="s">
+        <v>91</v>
+      </c>
+      <c r="B4" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="20">
+        <v>0</v>
+      </c>
+      <c r="E4" s="20">
+        <v>0.85</v>
+      </c>
+      <c r="F4" s="20">
+        <v>0</v>
+      </c>
+      <c r="G4" s="20">
+        <v>670000</v>
+      </c>
+      <c r="H4" s="21">
+        <v>13000</v>
+      </c>
+      <c r="I4" s="20">
+        <v>2.9</v>
+      </c>
+      <c r="J4" s="20">
+        <v>20</v>
+      </c>
+      <c r="K4" s="21">
+        <v>1</v>
+      </c>
+      <c r="L4" s="20">
+        <v>0</v>
+      </c>
+      <c r="M4" s="39">
+        <v>0</v>
+      </c>
+      <c r="N4"/>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5" s="20" t="s">
         <v>92</v>
       </c>
-      <c r="B3" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="21" t="s">
+      <c r="B5" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="20">
+        <v>0</v>
+      </c>
+      <c r="E5" s="21">
+        <v>0.87</v>
+      </c>
+      <c r="F5" s="20">
+        <v>0</v>
+      </c>
+      <c r="G5" s="20">
+        <v>700000</v>
+      </c>
+      <c r="H5" s="21">
+        <v>13000</v>
+      </c>
+      <c r="I5" s="20">
+        <v>3</v>
+      </c>
+      <c r="J5" s="21">
+        <v>20</v>
+      </c>
+      <c r="K5" s="21">
+        <v>1</v>
+      </c>
+      <c r="L5" s="20">
+        <v>0</v>
+      </c>
+      <c r="M5" s="39">
+        <v>0</v>
+      </c>
+      <c r="N5"/>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A6" s="20" t="s">
+        <v>93</v>
+      </c>
+      <c r="B6" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="C6" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" s="20">
+        <v>0</v>
+      </c>
+      <c r="E6" s="21">
+        <v>0.83</v>
+      </c>
+      <c r="F6" s="20">
+        <v>0</v>
+      </c>
+      <c r="G6" s="20">
+        <v>750000</v>
+      </c>
+      <c r="H6" s="21">
+        <v>13000</v>
+      </c>
+      <c r="I6" s="20">
+        <v>3.1</v>
+      </c>
+      <c r="J6" s="21">
+        <v>20</v>
+      </c>
+      <c r="K6" s="21">
+        <v>1</v>
+      </c>
+      <c r="L6" s="20">
+        <v>0</v>
+      </c>
+      <c r="M6" s="39">
+        <v>0</v>
+      </c>
+      <c r="N6"/>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A7" s="20" t="s">
+        <v>94</v>
+      </c>
+      <c r="B7" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="C7" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" s="20">
+        <v>0</v>
+      </c>
+      <c r="E7" s="20">
+        <v>0.81</v>
+      </c>
+      <c r="F7" s="20">
+        <v>0</v>
+      </c>
+      <c r="G7" s="20">
+        <v>1200000</v>
+      </c>
+      <c r="H7" s="20">
+        <v>230000</v>
+      </c>
+      <c r="I7" s="20">
+        <v>0.5</v>
+      </c>
+      <c r="J7" s="20">
+        <v>20</v>
+      </c>
+      <c r="K7" s="21">
+        <v>0.5</v>
+      </c>
+      <c r="L7" s="20">
+        <v>0</v>
+      </c>
+      <c r="M7" s="39">
+        <v>0</v>
+      </c>
+      <c r="N7"/>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A8" s="20" t="s">
+        <v>95</v>
+      </c>
+      <c r="B8" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="C8" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8" s="20">
+        <v>0</v>
+      </c>
+      <c r="E8" s="20">
+        <v>0.99</v>
+      </c>
+      <c r="F8" s="20">
+        <v>0</v>
+      </c>
+      <c r="G8" s="20">
+        <v>150000</v>
+      </c>
+      <c r="H8" s="20">
+        <v>2000</v>
+      </c>
+      <c r="I8" s="20">
+        <v>0.5</v>
+      </c>
+      <c r="J8" s="20">
+        <v>20</v>
+      </c>
+      <c r="K8" s="21">
+        <v>0.5</v>
+      </c>
+      <c r="L8" s="20">
+        <v>0</v>
+      </c>
+      <c r="M8" s="39">
+        <v>0</v>
+      </c>
+      <c r="N8"/>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A9" s="20" t="s">
+        <v>96</v>
+      </c>
+      <c r="B9" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="C9" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9" s="20">
+        <v>0</v>
+      </c>
+      <c r="E9" s="20">
+        <v>0</v>
+      </c>
+      <c r="F9" s="20">
+        <v>0</v>
+      </c>
+      <c r="G9" s="20">
+        <v>1600000</v>
+      </c>
+      <c r="H9" s="20">
+        <v>35000</v>
+      </c>
+      <c r="I9" s="20">
+        <v>0</v>
+      </c>
+      <c r="J9" s="20">
+        <v>30</v>
+      </c>
+      <c r="K9" s="21">
+        <v>1</v>
+      </c>
+      <c r="L9" s="20">
+        <v>0</v>
+      </c>
+      <c r="M9" s="39">
+        <v>0</v>
+      </c>
+      <c r="N9"/>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A10" s="20" t="s">
+        <v>118</v>
+      </c>
+      <c r="B10" s="20" t="s">
+        <v>81</v>
+      </c>
+      <c r="C10" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="21">
-        <v>0</v>
-      </c>
-      <c r="E3" s="21">
-        <v>0.9</v>
-      </c>
-      <c r="F3" s="21">
-        <v>0</v>
-      </c>
-      <c r="G3" s="21">
-        <v>100000</v>
-      </c>
-      <c r="H3" s="21">
-        <v>4000</v>
-      </c>
-      <c r="I3" s="21">
+      <c r="D10" s="20">
+        <v>0</v>
+      </c>
+      <c r="E10" s="21">
+        <v>0.46</v>
+      </c>
+      <c r="F10" s="20">
+        <v>0.37</v>
+      </c>
+      <c r="G10" s="20">
+        <v>875000</v>
+      </c>
+      <c r="H10" s="20">
+        <v>23000</v>
+      </c>
+      <c r="I10" s="20">
+        <v>1.7</v>
+      </c>
+      <c r="J10" s="20">
+        <v>25</v>
+      </c>
+      <c r="K10" s="21">
+        <v>0</v>
+      </c>
+      <c r="L10" s="20">
+        <v>0</v>
+      </c>
+      <c r="M10" s="39">
+        <v>100</v>
+      </c>
+      <c r="N10"/>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A11" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="B11" s="20" t="s">
+        <v>81</v>
+      </c>
+      <c r="C11" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="D11" s="20">
+        <v>0</v>
+      </c>
+      <c r="E11" s="21">
+        <v>0.35</v>
+      </c>
+      <c r="F11" s="20">
         <v>0.5</v>
       </c>
-      <c r="J3" s="21">
+      <c r="G11" s="20">
+        <v>1500000</v>
+      </c>
+      <c r="H11" s="20">
+        <v>34000</v>
+      </c>
+      <c r="I11" s="20">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="J11" s="20">
         <v>25</v>
       </c>
-      <c r="K3" s="22">
-        <v>0</v>
-      </c>
-      <c r="L3" s="21">
-        <v>0</v>
-      </c>
-      <c r="N3"/>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A4" s="21" t="s">
-        <v>93</v>
-      </c>
-      <c r="B4" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="C4" s="21" t="s">
+      <c r="K11" s="21">
+        <v>0</v>
+      </c>
+      <c r="L11" s="20">
+        <v>0</v>
+      </c>
+      <c r="M11" s="39">
+        <v>100</v>
+      </c>
+      <c r="N11"/>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A12" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="B12" s="22" t="s">
+        <v>80</v>
+      </c>
+      <c r="C12" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="D12" s="20">
+        <v>0</v>
+      </c>
+      <c r="E12" s="21">
+        <v>0.36</v>
+      </c>
+      <c r="F12" s="20">
+        <v>0.5</v>
+      </c>
+      <c r="G12" s="20">
+        <v>1300000</v>
+      </c>
+      <c r="H12" s="20">
+        <v>34000</v>
+      </c>
+      <c r="I12" s="20">
+        <v>4.5</v>
+      </c>
+      <c r="J12" s="20">
+        <v>25</v>
+      </c>
+      <c r="K12" s="21">
+        <v>0</v>
+      </c>
+      <c r="L12" s="20">
+        <v>0</v>
+      </c>
+      <c r="M12" s="39">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A13" s="23" t="s">
+        <v>140</v>
+      </c>
+      <c r="B13" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="C13" s="23" t="s">
+        <v>38</v>
+      </c>
+      <c r="D13" s="23">
+        <v>0</v>
+      </c>
+      <c r="E13" s="24">
+        <v>0.8</v>
+      </c>
+      <c r="F13" s="23">
+        <v>0</v>
+      </c>
+      <c r="G13" s="23">
+        <v>550000</v>
+      </c>
+      <c r="H13" s="23">
+        <v>10000</v>
+      </c>
+      <c r="I13" s="23">
+        <v>0.5</v>
+      </c>
+      <c r="J13" s="23">
+        <v>20</v>
+      </c>
+      <c r="K13" s="23">
+        <v>1</v>
+      </c>
+      <c r="L13" s="24">
+        <v>0</v>
+      </c>
+      <c r="M13" s="39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A14" s="16" t="s">
+        <v>115</v>
+      </c>
+      <c r="B14" s="16" t="s">
+        <v>76</v>
+      </c>
+      <c r="C14" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="D14" s="16">
+        <v>0</v>
+      </c>
+      <c r="E14" s="17">
+        <v>4</v>
+      </c>
+      <c r="F14" s="32">
+        <v>0</v>
+      </c>
+      <c r="G14" s="32">
+        <v>510000</v>
+      </c>
+      <c r="H14" s="32">
+        <v>10000</v>
+      </c>
+      <c r="I14" s="32">
+        <v>0.5</v>
+      </c>
+      <c r="J14" s="32">
+        <v>25</v>
+      </c>
+      <c r="K14" s="33">
+        <v>0.75</v>
+      </c>
+      <c r="L14" s="32">
+        <v>0</v>
+      </c>
+      <c r="M14" s="39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A15" s="16" t="s">
+        <v>114</v>
+      </c>
+      <c r="B15" s="16" t="s">
+        <v>76</v>
+      </c>
+      <c r="C15" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="D15" s="16">
+        <v>0</v>
+      </c>
+      <c r="E15" s="17">
+        <v>4</v>
+      </c>
+      <c r="F15" s="34">
+        <v>0</v>
+      </c>
+      <c r="G15" s="34">
+        <v>510000</v>
+      </c>
+      <c r="H15" s="34">
+        <v>10000</v>
+      </c>
+      <c r="I15" s="34">
+        <v>0.5</v>
+      </c>
+      <c r="J15" s="34">
+        <v>25</v>
+      </c>
+      <c r="K15" s="35">
+        <v>0.75</v>
+      </c>
+      <c r="L15" s="34">
+        <v>0</v>
+      </c>
+      <c r="M15" s="39">
+        <v>0</v>
+      </c>
+      <c r="N15"/>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A16" s="16" t="s">
+        <v>112</v>
+      </c>
+      <c r="B16" s="16" t="s">
+        <v>76</v>
+      </c>
+      <c r="C16" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="D16" s="16">
+        <v>0</v>
+      </c>
+      <c r="E16" s="17">
+        <v>4</v>
+      </c>
+      <c r="F16" s="36">
+        <v>0</v>
+      </c>
+      <c r="G16" s="36">
+        <v>510000</v>
+      </c>
+      <c r="H16" s="36">
+        <v>10000</v>
+      </c>
+      <c r="I16" s="36">
+        <v>0.5</v>
+      </c>
+      <c r="J16" s="36">
+        <v>25</v>
+      </c>
+      <c r="K16" s="37">
+        <v>0.75</v>
+      </c>
+      <c r="L16" s="36">
+        <v>0</v>
+      </c>
+      <c r="M16" s="39">
+        <v>0</v>
+      </c>
+      <c r="N16"/>
+    </row>
+    <row r="17" spans="1:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="16" t="s">
+        <v>113</v>
+      </c>
+      <c r="B17" s="16" t="s">
+        <v>76</v>
+      </c>
+      <c r="C17" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="D17" s="16">
+        <v>0</v>
+      </c>
+      <c r="E17" s="17">
+        <v>4</v>
+      </c>
+      <c r="F17" s="39">
+        <v>0</v>
+      </c>
+      <c r="G17" s="39">
+        <v>510000</v>
+      </c>
+      <c r="H17" s="39">
+        <v>10000</v>
+      </c>
+      <c r="I17" s="39">
+        <v>0.5</v>
+      </c>
+      <c r="J17" s="39">
+        <v>25</v>
+      </c>
+      <c r="K17" s="40">
+        <v>0.75</v>
+      </c>
+      <c r="L17" s="39">
+        <v>0</v>
+      </c>
+      <c r="M17" s="39">
+        <v>0</v>
+      </c>
+      <c r="N17"/>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A18" s="44" t="s">
+        <v>128</v>
+      </c>
+      <c r="B18" s="44" t="s">
+        <v>1</v>
+      </c>
+      <c r="C18" s="44" t="s">
+        <v>8</v>
+      </c>
+      <c r="D18" s="44">
+        <v>0</v>
+      </c>
+      <c r="E18" s="44">
+        <v>0.75</v>
+      </c>
+      <c r="F18" s="44">
+        <v>0</v>
+      </c>
+      <c r="G18" s="44">
+        <v>1200000</v>
+      </c>
+      <c r="H18" s="44">
+        <v>54000</v>
+      </c>
+      <c r="I18" s="44">
+        <v>5.6</v>
+      </c>
+      <c r="J18" s="44">
+        <v>20</v>
+      </c>
+      <c r="K18" s="44">
+        <v>0</v>
+      </c>
+      <c r="L18" s="44">
+        <v>0</v>
+      </c>
+      <c r="M18" s="44">
+        <v>100</v>
+      </c>
+      <c r="N18"/>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A19" s="44" t="s">
+        <v>130</v>
+      </c>
+      <c r="B19" s="44" t="s">
+        <v>77</v>
+      </c>
+      <c r="C19" s="44" t="s">
+        <v>9</v>
+      </c>
+      <c r="D19" s="44">
+        <v>0</v>
+      </c>
+      <c r="E19" s="44">
+        <v>0</v>
+      </c>
+      <c r="F19" s="44">
+        <v>0</v>
+      </c>
+      <c r="G19" s="44">
+        <v>0</v>
+      </c>
+      <c r="H19" s="44">
+        <v>0</v>
+      </c>
+      <c r="I19" s="44">
+        <v>0</v>
+      </c>
+      <c r="J19" s="44">
+        <v>0</v>
+      </c>
+      <c r="K19" s="44">
+        <v>0</v>
+      </c>
+      <c r="L19" s="44">
+        <v>0</v>
+      </c>
+      <c r="M19" s="44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A20" s="44" t="s">
+        <v>136</v>
+      </c>
+      <c r="B20" s="44" t="s">
+        <v>78</v>
+      </c>
+      <c r="C20" s="44" t="s">
+        <v>122</v>
+      </c>
+      <c r="D20" s="44">
+        <v>0</v>
+      </c>
+      <c r="E20" s="44">
+        <v>0</v>
+      </c>
+      <c r="F20" s="44">
+        <v>0</v>
+      </c>
+      <c r="G20" s="44">
+        <v>0</v>
+      </c>
+      <c r="H20" s="44">
+        <v>0</v>
+      </c>
+      <c r="I20" s="44">
+        <v>0</v>
+      </c>
+      <c r="J20" s="44">
+        <v>0</v>
+      </c>
+      <c r="K20" s="44">
+        <v>0</v>
+      </c>
+      <c r="L20" s="44">
+        <v>0</v>
+      </c>
+      <c r="M20" s="44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A21" s="44" t="s">
+        <v>129</v>
+      </c>
+      <c r="B21" s="44" t="s">
+        <v>79</v>
+      </c>
+      <c r="C21" s="44" t="s">
+        <v>123</v>
+      </c>
+      <c r="D21" s="44">
+        <v>0</v>
+      </c>
+      <c r="E21" s="44">
+        <v>0.1</v>
+      </c>
+      <c r="F21" s="44">
+        <v>0</v>
+      </c>
+      <c r="G21" s="44">
+        <v>0</v>
+      </c>
+      <c r="H21" s="44">
+        <v>0</v>
+      </c>
+      <c r="I21" s="44">
+        <v>0</v>
+      </c>
+      <c r="J21" s="44">
+        <v>0</v>
+      </c>
+      <c r="K21" s="44">
+        <v>0</v>
+      </c>
+      <c r="L21" s="44">
+        <v>0</v>
+      </c>
+      <c r="M21" s="44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A22" s="44" t="s">
+        <v>131</v>
+      </c>
+      <c r="B22" s="44" t="s">
+        <v>81</v>
+      </c>
+      <c r="C22" s="44" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="21">
-        <v>0</v>
-      </c>
-      <c r="E4" s="21">
-        <v>0.85</v>
-      </c>
-      <c r="F4" s="21">
-        <v>0</v>
-      </c>
-      <c r="G4" s="21">
-        <v>670000</v>
-      </c>
-      <c r="H4" s="22">
-        <v>13000</v>
-      </c>
-      <c r="I4" s="21">
-        <v>2.9</v>
-      </c>
-      <c r="J4" s="21">
+      <c r="D22" s="44">
+        <v>0</v>
+      </c>
+      <c r="E22" s="44">
+        <v>0.64</v>
+      </c>
+      <c r="F22" s="44">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="G22" s="44">
+        <v>4000000</v>
+      </c>
+      <c r="H22" s="44">
+        <v>29000</v>
+      </c>
+      <c r="I22" s="44">
+        <v>3.9</v>
+      </c>
+      <c r="J22" s="44">
+        <v>30</v>
+      </c>
+      <c r="K22" s="44">
+        <v>1</v>
+      </c>
+      <c r="L22" s="44">
+        <v>0</v>
+      </c>
+      <c r="M22" s="44">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A23" s="44" t="s">
+        <v>132</v>
+      </c>
+      <c r="B23" s="44" t="s">
+        <v>81</v>
+      </c>
+      <c r="C23" s="44" t="s">
+        <v>5</v>
+      </c>
+      <c r="D23" s="44">
+        <v>0</v>
+      </c>
+      <c r="E23" s="44">
+        <v>0.62</v>
+      </c>
+      <c r="F23" s="44">
+        <v>0.25</v>
+      </c>
+      <c r="G23" s="44">
+        <v>6000000</v>
+      </c>
+      <c r="H23" s="44">
+        <v>150000</v>
+      </c>
+      <c r="I23" s="44">
+        <v>0</v>
+      </c>
+      <c r="J23" s="44">
         <v>20</v>
       </c>
-      <c r="K4" s="22">
+      <c r="K23" s="44">
         <v>1</v>
       </c>
-      <c r="L4" s="21">
-        <v>0</v>
-      </c>
-      <c r="N4"/>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A5" s="21" t="s">
-        <v>94</v>
-      </c>
-      <c r="B5" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="C5" s="21" t="s">
-        <v>6</v>
-      </c>
-      <c r="D5" s="21">
-        <v>0</v>
-      </c>
-      <c r="E5" s="22">
-        <v>0.87</v>
-      </c>
-      <c r="F5" s="21">
-        <v>0</v>
-      </c>
-      <c r="G5" s="21">
-        <v>700000</v>
-      </c>
-      <c r="H5" s="22">
-        <v>13000</v>
-      </c>
-      <c r="I5" s="21">
-        <v>3</v>
-      </c>
-      <c r="J5" s="22">
+      <c r="L23" s="44">
+        <v>0</v>
+      </c>
+      <c r="M23" s="44">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A24" s="44" t="s">
+        <v>133</v>
+      </c>
+      <c r="B24" s="44" t="s">
+        <v>81</v>
+      </c>
+      <c r="C24" s="44" t="s">
+        <v>7</v>
+      </c>
+      <c r="D24" s="44">
+        <v>0</v>
+      </c>
+      <c r="E24" s="44">
+        <v>0.64</v>
+      </c>
+      <c r="F24" s="44">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="G24" s="44">
+        <v>4000000</v>
+      </c>
+      <c r="H24" s="44">
+        <v>40000</v>
+      </c>
+      <c r="I24" s="44">
+        <v>6.4</v>
+      </c>
+      <c r="J24" s="44">
+        <v>25</v>
+      </c>
+      <c r="K24" s="44">
+        <v>1</v>
+      </c>
+      <c r="L24" s="44">
+        <v>0</v>
+      </c>
+      <c r="M24" s="44">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A25" s="44" t="s">
+        <v>134</v>
+      </c>
+      <c r="B25" s="44" t="s">
+        <v>81</v>
+      </c>
+      <c r="C25" s="44" t="s">
+        <v>7</v>
+      </c>
+      <c r="D25" s="44">
+        <v>0</v>
+      </c>
+      <c r="E25" s="44">
+        <v>0.62</v>
+      </c>
+      <c r="F25" s="44">
+        <v>0.3</v>
+      </c>
+      <c r="G25" s="44">
+        <v>6000000</v>
+      </c>
+      <c r="H25" s="44">
+        <v>150000</v>
+      </c>
+      <c r="I25" s="44">
+        <v>0</v>
+      </c>
+      <c r="J25" s="44">
         <v>20</v>
       </c>
-      <c r="K5" s="22">
+      <c r="K25" s="44">
         <v>1</v>
       </c>
-      <c r="L5" s="21">
-        <v>0</v>
-      </c>
-      <c r="N5"/>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A6" s="21" t="s">
-        <v>95</v>
-      </c>
-      <c r="B6" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="C6" s="21" t="s">
-        <v>7</v>
-      </c>
-      <c r="D6" s="21">
-        <v>0</v>
-      </c>
-      <c r="E6" s="22">
-        <v>0.83</v>
-      </c>
-      <c r="F6" s="21">
-        <v>0</v>
-      </c>
-      <c r="G6" s="21">
-        <v>750000</v>
-      </c>
-      <c r="H6" s="22">
-        <v>13000</v>
-      </c>
-      <c r="I6" s="21">
-        <v>3.1</v>
-      </c>
-      <c r="J6" s="22">
+      <c r="L25" s="44">
+        <v>0</v>
+      </c>
+      <c r="M25" s="44">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A26" s="44" t="s">
+        <v>135</v>
+      </c>
+      <c r="B26" s="44" t="s">
+        <v>81</v>
+      </c>
+      <c r="C26" s="44" t="s">
+        <v>8</v>
+      </c>
+      <c r="D26" s="44">
+        <v>0</v>
+      </c>
+      <c r="E26" s="44">
+        <v>0.62</v>
+      </c>
+      <c r="F26" s="44">
+        <v>0.24</v>
+      </c>
+      <c r="G26" s="44">
+        <v>8500000</v>
+      </c>
+      <c r="H26" s="44">
+        <v>150000</v>
+      </c>
+      <c r="I26" s="44">
+        <v>0</v>
+      </c>
+      <c r="J26" s="44">
         <v>20</v>
       </c>
-      <c r="K6" s="22">
+      <c r="K26" s="44">
         <v>1</v>
       </c>
-      <c r="L6" s="21">
-        <v>0</v>
-      </c>
-      <c r="N6"/>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A7" s="21" t="s">
-        <v>96</v>
-      </c>
-      <c r="B7" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="C7" s="21" t="s">
+      <c r="L26" s="44">
+        <v>0</v>
+      </c>
+      <c r="M26" s="44">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A27" s="44" t="s">
+        <v>137</v>
+      </c>
+      <c r="B27" s="44" t="s">
+        <v>80</v>
+      </c>
+      <c r="C27" s="44" t="s">
+        <v>121</v>
+      </c>
+      <c r="D27" s="44">
+        <v>0</v>
+      </c>
+      <c r="E27" s="44">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="F27" s="44">
+        <v>0.2</v>
+      </c>
+      <c r="G27" s="44">
+        <v>5000000</v>
+      </c>
+      <c r="H27" s="44">
+        <v>32000</v>
+      </c>
+      <c r="I27" s="44">
+        <v>26</v>
+      </c>
+      <c r="J27" s="44">
+        <v>15</v>
+      </c>
+      <c r="K27" s="44">
+        <v>1</v>
+      </c>
+      <c r="L27" s="44">
+        <v>0</v>
+      </c>
+      <c r="M27" s="44">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A28" s="44" t="s">
+        <v>138</v>
+      </c>
+      <c r="B28" s="44" t="s">
+        <v>80</v>
+      </c>
+      <c r="C28" s="44" t="s">
+        <v>4</v>
+      </c>
+      <c r="D28" s="44">
+        <v>0</v>
+      </c>
+      <c r="E28" s="44">
+        <v>0.45</v>
+      </c>
+      <c r="F28" s="44">
+        <v>0.44</v>
+      </c>
+      <c r="G28" s="44">
+        <v>1000000</v>
+      </c>
+      <c r="H28" s="44">
+        <v>10000</v>
+      </c>
+      <c r="I28" s="44">
+        <v>5.4</v>
+      </c>
+      <c r="J28" s="44">
+        <v>25</v>
+      </c>
+      <c r="K28" s="44">
+        <v>1</v>
+      </c>
+      <c r="L28" s="44">
+        <v>0</v>
+      </c>
+      <c r="M28" s="44">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A29" s="44" t="s">
+        <v>139</v>
+      </c>
+      <c r="B29" s="44" t="s">
+        <v>80</v>
+      </c>
+      <c r="C29" s="44" t="s">
+        <v>121</v>
+      </c>
+      <c r="D29" s="44">
+        <v>0</v>
+      </c>
+      <c r="E29" s="44">
+        <v>0.45</v>
+      </c>
+      <c r="F29" s="44">
+        <v>0.4</v>
+      </c>
+      <c r="G29" s="44">
+        <v>1000000</v>
+      </c>
+      <c r="H29" s="44">
+        <v>10000</v>
+      </c>
+      <c r="I29" s="44">
         <v>8</v>
       </c>
-      <c r="D7" s="21">
-        <v>0</v>
-      </c>
-      <c r="E7" s="21">
-        <v>0.81</v>
-      </c>
-      <c r="F7" s="21">
-        <v>0</v>
-      </c>
-      <c r="G7" s="21">
-        <v>1200000</v>
-      </c>
-      <c r="H7" s="21">
-        <v>230000</v>
-      </c>
-      <c r="I7" s="21">
-        <v>0.5</v>
-      </c>
-      <c r="J7" s="21">
-        <v>20</v>
-      </c>
-      <c r="K7" s="22">
-        <v>0.5</v>
-      </c>
-      <c r="L7" s="21">
-        <v>0</v>
-      </c>
-      <c r="N7"/>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A8" s="21" t="s">
-        <v>97</v>
-      </c>
-      <c r="B8" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="C8" s="21" t="s">
-        <v>9</v>
-      </c>
-      <c r="D8" s="21">
-        <v>0</v>
-      </c>
-      <c r="E8" s="21">
-        <v>0.99</v>
-      </c>
-      <c r="F8" s="21">
-        <v>0</v>
-      </c>
-      <c r="G8" s="21">
-        <v>150000</v>
-      </c>
-      <c r="H8" s="21">
-        <v>2000</v>
-      </c>
-      <c r="I8" s="21">
-        <v>0.5</v>
-      </c>
-      <c r="J8" s="21">
-        <v>20</v>
-      </c>
-      <c r="K8" s="22">
-        <v>0.5</v>
-      </c>
-      <c r="L8" s="21">
-        <v>0</v>
-      </c>
-      <c r="N8"/>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A9" s="21" t="s">
-        <v>98</v>
-      </c>
-      <c r="B9" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="C9" s="21" t="s">
-        <v>10</v>
-      </c>
-      <c r="D9" s="21">
-        <v>0</v>
-      </c>
-      <c r="E9" s="21">
-        <v>0</v>
-      </c>
-      <c r="F9" s="21">
-        <v>0</v>
-      </c>
-      <c r="G9" s="21">
-        <v>1600000</v>
-      </c>
-      <c r="H9" s="21">
-        <v>35000</v>
-      </c>
-      <c r="I9" s="21">
-        <v>0</v>
-      </c>
-      <c r="J9" s="21">
-        <v>30</v>
-      </c>
-      <c r="K9" s="22">
+      <c r="J29" s="44">
+        <v>25</v>
+      </c>
+      <c r="K29" s="44">
         <v>1</v>
       </c>
-      <c r="L9" s="21">
-        <v>0</v>
-      </c>
-      <c r="N9"/>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A10" s="21" t="s">
-        <v>120</v>
-      </c>
-      <c r="B10" s="21" t="s">
-        <v>83</v>
-      </c>
-      <c r="C10" s="21" t="s">
-        <v>4</v>
-      </c>
-      <c r="D10" s="21">
-        <v>0</v>
-      </c>
-      <c r="E10" s="22">
-        <v>0.46</v>
-      </c>
-      <c r="F10" s="21">
-        <v>0.37</v>
-      </c>
-      <c r="G10" s="21">
-        <v>875000</v>
-      </c>
-      <c r="H10" s="21">
-        <v>23000</v>
-      </c>
-      <c r="I10" s="21">
-        <v>1.7</v>
-      </c>
-      <c r="J10" s="21">
-        <v>25</v>
-      </c>
-      <c r="K10" s="22">
-        <v>0</v>
-      </c>
-      <c r="L10" s="21">
-        <v>0</v>
-      </c>
-      <c r="N10"/>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A11" s="21" t="s">
-        <v>2</v>
-      </c>
-      <c r="B11" s="21" t="s">
-        <v>83</v>
-      </c>
-      <c r="C11" s="21" t="s">
-        <v>4</v>
-      </c>
-      <c r="D11" s="21">
-        <v>0</v>
-      </c>
-      <c r="E11" s="22">
-        <v>0.35</v>
-      </c>
-      <c r="F11" s="21">
-        <v>0.5</v>
-      </c>
-      <c r="G11" s="21">
-        <v>1500000</v>
-      </c>
-      <c r="H11" s="21">
-        <v>34000</v>
-      </c>
-      <c r="I11" s="21">
-        <v>4.5999999999999996</v>
-      </c>
-      <c r="J11" s="21">
-        <v>25</v>
-      </c>
-      <c r="K11" s="22">
-        <v>0</v>
-      </c>
-      <c r="L11" s="21">
-        <v>0</v>
-      </c>
-      <c r="N11"/>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A12" s="21" t="s">
-        <v>3</v>
-      </c>
-      <c r="B12" s="23" t="s">
-        <v>82</v>
-      </c>
-      <c r="C12" s="21" t="s">
-        <v>4</v>
-      </c>
-      <c r="D12" s="21">
-        <v>0</v>
-      </c>
-      <c r="E12" s="22">
-        <v>0.36</v>
-      </c>
-      <c r="F12" s="21">
-        <v>0.5</v>
-      </c>
-      <c r="G12" s="21">
-        <v>1300000</v>
-      </c>
-      <c r="H12" s="21">
-        <v>34000</v>
-      </c>
-      <c r="I12" s="21">
-        <v>4.5</v>
-      </c>
-      <c r="J12" s="21">
-        <v>25</v>
-      </c>
-      <c r="K12" s="22">
-        <v>0</v>
-      </c>
-      <c r="L12" s="21">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A13" s="24" t="s">
-        <v>142</v>
-      </c>
-      <c r="B13" s="24" t="s">
-        <v>57</v>
-      </c>
-      <c r="C13" s="24" t="s">
-        <v>38</v>
-      </c>
-      <c r="D13" s="24">
-        <v>0</v>
-      </c>
-      <c r="E13" s="25">
-        <v>0.8</v>
-      </c>
-      <c r="F13" s="24">
-        <v>0</v>
-      </c>
-      <c r="G13" s="24">
-        <v>550000</v>
-      </c>
-      <c r="H13" s="24">
-        <v>10000</v>
-      </c>
-      <c r="I13" s="24">
-        <v>0.5</v>
-      </c>
-      <c r="J13" s="24">
-        <v>20</v>
-      </c>
-      <c r="K13" s="24">
-        <v>1</v>
-      </c>
-      <c r="L13" s="25">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A14" s="17" t="s">
-        <v>117</v>
-      </c>
-      <c r="B14" s="17" t="s">
-        <v>78</v>
-      </c>
-      <c r="C14" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="D14" s="17">
-        <v>0</v>
-      </c>
-      <c r="E14" s="18">
-        <v>4</v>
-      </c>
-      <c r="F14" s="33">
-        <v>0</v>
-      </c>
-      <c r="G14" s="33">
-        <v>510000</v>
-      </c>
-      <c r="H14" s="33">
-        <v>10000</v>
-      </c>
-      <c r="I14" s="33">
-        <v>0.5</v>
-      </c>
-      <c r="J14" s="33">
-        <v>25</v>
-      </c>
-      <c r="K14" s="34">
-        <v>0.75</v>
-      </c>
-      <c r="L14" s="33">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A15" s="17" t="s">
-        <v>116</v>
-      </c>
-      <c r="B15" s="17" t="s">
-        <v>78</v>
-      </c>
-      <c r="C15" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="D15" s="17">
-        <v>0</v>
-      </c>
-      <c r="E15" s="18">
-        <v>4</v>
-      </c>
-      <c r="F15" s="35">
-        <v>0</v>
-      </c>
-      <c r="G15" s="35">
-        <v>510000</v>
-      </c>
-      <c r="H15" s="35">
-        <v>10000</v>
-      </c>
-      <c r="I15" s="35">
-        <v>0.5</v>
-      </c>
-      <c r="J15" s="35">
-        <v>25</v>
-      </c>
-      <c r="K15" s="36">
-        <v>0.75</v>
-      </c>
-      <c r="L15" s="35">
-        <v>0</v>
-      </c>
-      <c r="N15"/>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A16" s="17" t="s">
-        <v>114</v>
-      </c>
-      <c r="B16" s="17" t="s">
-        <v>78</v>
-      </c>
-      <c r="C16" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="D16" s="17">
-        <v>0</v>
-      </c>
-      <c r="E16" s="18">
-        <v>4</v>
-      </c>
-      <c r="F16" s="37">
-        <v>0</v>
-      </c>
-      <c r="G16" s="37">
-        <v>510000</v>
-      </c>
-      <c r="H16" s="37">
-        <v>10000</v>
-      </c>
-      <c r="I16" s="37">
-        <v>0.5</v>
-      </c>
-      <c r="J16" s="37">
-        <v>25</v>
-      </c>
-      <c r="K16" s="38">
-        <v>0.75</v>
-      </c>
-      <c r="L16" s="37">
-        <v>0</v>
-      </c>
-      <c r="N16"/>
-    </row>
-    <row r="17" spans="1:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="17" t="s">
-        <v>115</v>
-      </c>
-      <c r="B17" s="17" t="s">
-        <v>78</v>
-      </c>
-      <c r="C17" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="D17" s="17">
-        <v>0</v>
-      </c>
-      <c r="E17" s="18">
-        <v>4</v>
-      </c>
-      <c r="F17" s="40">
-        <v>0</v>
-      </c>
-      <c r="G17" s="40">
-        <v>510000</v>
-      </c>
-      <c r="H17" s="40">
-        <v>10000</v>
-      </c>
-      <c r="I17" s="40">
-        <v>0.5</v>
-      </c>
-      <c r="J17" s="40">
-        <v>25</v>
-      </c>
-      <c r="K17" s="41">
-        <v>0.75</v>
-      </c>
-      <c r="L17" s="40">
-        <v>0</v>
-      </c>
-      <c r="N17"/>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A18" s="45" t="s">
-        <v>130</v>
-      </c>
-      <c r="B18" s="45" t="s">
-        <v>1</v>
-      </c>
-      <c r="C18" s="45" t="s">
-        <v>8</v>
-      </c>
-      <c r="D18" s="45">
-        <v>0</v>
-      </c>
-      <c r="E18" s="45">
-        <v>0.75</v>
-      </c>
-      <c r="F18" s="45">
-        <v>0.3</v>
-      </c>
-      <c r="G18" s="45">
-        <v>1200000</v>
-      </c>
-      <c r="H18" s="45">
-        <v>54000</v>
-      </c>
-      <c r="I18" s="45">
-        <v>5.6</v>
-      </c>
-      <c r="J18" s="45">
-        <v>20</v>
-      </c>
-      <c r="K18" s="45">
-        <v>0</v>
-      </c>
-      <c r="L18" s="45">
-        <v>0</v>
-      </c>
-      <c r="N18"/>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A19" s="45" t="s">
-        <v>132</v>
-      </c>
-      <c r="B19" s="45" t="s">
-        <v>79</v>
-      </c>
-      <c r="C19" s="45" t="s">
-        <v>9</v>
-      </c>
-      <c r="D19" s="45">
-        <v>0</v>
-      </c>
-      <c r="E19" s="45">
-        <v>0</v>
-      </c>
-      <c r="F19" s="45">
-        <v>0</v>
-      </c>
-      <c r="G19" s="45">
-        <v>0</v>
-      </c>
-      <c r="H19" s="45">
-        <v>0</v>
-      </c>
-      <c r="I19" s="45">
-        <v>0</v>
-      </c>
-      <c r="J19" s="45">
-        <v>0</v>
-      </c>
-      <c r="K19" s="45">
-        <v>0</v>
-      </c>
-      <c r="L19" s="45">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A20" s="45" t="s">
-        <v>138</v>
-      </c>
-      <c r="B20" s="45" t="s">
-        <v>80</v>
-      </c>
-      <c r="C20" s="45" t="s">
-        <v>124</v>
-      </c>
-      <c r="D20" s="45">
-        <v>0</v>
-      </c>
-      <c r="E20" s="45">
-        <v>0</v>
-      </c>
-      <c r="F20" s="45">
-        <v>0</v>
-      </c>
-      <c r="G20" s="45">
-        <v>0</v>
-      </c>
-      <c r="H20" s="45">
-        <v>0</v>
-      </c>
-      <c r="I20" s="45">
-        <v>0</v>
-      </c>
-      <c r="J20" s="45">
-        <v>0</v>
-      </c>
-      <c r="K20" s="45">
-        <v>0</v>
-      </c>
-      <c r="L20" s="45">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A21" s="45" t="s">
-        <v>131</v>
-      </c>
-      <c r="B21" s="45" t="s">
-        <v>81</v>
-      </c>
-      <c r="C21" s="45" t="s">
-        <v>125</v>
-      </c>
-      <c r="D21" s="45">
-        <v>0</v>
-      </c>
-      <c r="E21" s="45">
-        <v>0.1</v>
-      </c>
-      <c r="F21" s="45">
-        <v>0</v>
-      </c>
-      <c r="G21" s="45">
-        <v>0</v>
-      </c>
-      <c r="H21" s="45">
-        <v>0</v>
-      </c>
-      <c r="I21" s="45">
-        <v>0</v>
-      </c>
-      <c r="J21" s="45">
-        <v>0</v>
-      </c>
-      <c r="K21" s="45">
-        <v>0</v>
-      </c>
-      <c r="L21" s="45">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A22" s="45" t="s">
-        <v>133</v>
-      </c>
-      <c r="B22" s="45" t="s">
-        <v>83</v>
-      </c>
-      <c r="C22" s="45" t="s">
-        <v>5</v>
-      </c>
-      <c r="D22" s="45">
-        <v>0</v>
-      </c>
-      <c r="E22" s="45">
-        <v>0.64</v>
-      </c>
-      <c r="F22" s="45">
-        <v>0.28999999999999998</v>
-      </c>
-      <c r="G22" s="45">
-        <v>4000000</v>
-      </c>
-      <c r="H22" s="45">
-        <v>29000</v>
-      </c>
-      <c r="I22" s="45">
-        <v>3.9</v>
-      </c>
-      <c r="J22" s="45">
-        <v>30</v>
-      </c>
-      <c r="K22" s="45">
-        <v>1</v>
-      </c>
-      <c r="L22" s="45">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A23" s="45" t="s">
-        <v>134</v>
-      </c>
-      <c r="B23" s="45" t="s">
-        <v>83</v>
-      </c>
-      <c r="C23" s="45" t="s">
-        <v>5</v>
-      </c>
-      <c r="D23" s="45">
-        <v>0</v>
-      </c>
-      <c r="E23" s="45">
-        <v>0.62</v>
-      </c>
-      <c r="F23" s="45">
-        <v>0.25</v>
-      </c>
-      <c r="G23" s="45">
-        <v>6000000</v>
-      </c>
-      <c r="H23" s="45">
-        <v>150000</v>
-      </c>
-      <c r="I23" s="45">
-        <v>0</v>
-      </c>
-      <c r="J23" s="45">
-        <v>20</v>
-      </c>
-      <c r="K23" s="45">
-        <v>1</v>
-      </c>
-      <c r="L23" s="45">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A24" s="45" t="s">
-        <v>135</v>
-      </c>
-      <c r="B24" s="45" t="s">
-        <v>83</v>
-      </c>
-      <c r="C24" s="45" t="s">
-        <v>7</v>
-      </c>
-      <c r="D24" s="45">
-        <v>0</v>
-      </c>
-      <c r="E24" s="45">
-        <v>0.64</v>
-      </c>
-      <c r="F24" s="45">
-        <v>0.28999999999999998</v>
-      </c>
-      <c r="G24" s="45">
-        <v>4000000</v>
-      </c>
-      <c r="H24" s="45">
-        <v>40000</v>
-      </c>
-      <c r="I24" s="45">
-        <v>6.4</v>
-      </c>
-      <c r="J24" s="45">
-        <v>25</v>
-      </c>
-      <c r="K24" s="45">
-        <v>1</v>
-      </c>
-      <c r="L24" s="45">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A25" s="45" t="s">
-        <v>136</v>
-      </c>
-      <c r="B25" s="45" t="s">
-        <v>83</v>
-      </c>
-      <c r="C25" s="45" t="s">
-        <v>7</v>
-      </c>
-      <c r="D25" s="45">
-        <v>0</v>
-      </c>
-      <c r="E25" s="45">
-        <v>0.62</v>
-      </c>
-      <c r="F25" s="45">
-        <v>0.3</v>
-      </c>
-      <c r="G25" s="45">
-        <v>6000000</v>
-      </c>
-      <c r="H25" s="45">
-        <v>150000</v>
-      </c>
-      <c r="I25" s="45">
-        <v>0</v>
-      </c>
-      <c r="J25" s="45">
-        <v>20</v>
-      </c>
-      <c r="K25" s="45">
-        <v>1</v>
-      </c>
-      <c r="L25" s="45">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A26" s="45" t="s">
-        <v>137</v>
-      </c>
-      <c r="B26" s="45" t="s">
-        <v>83</v>
-      </c>
-      <c r="C26" s="45" t="s">
-        <v>8</v>
-      </c>
-      <c r="D26" s="45">
-        <v>0</v>
-      </c>
-      <c r="E26" s="45">
-        <v>0.62</v>
-      </c>
-      <c r="F26" s="45">
-        <v>0.24</v>
-      </c>
-      <c r="G26" s="45">
-        <v>8500000</v>
-      </c>
-      <c r="H26" s="45">
-        <v>150000</v>
-      </c>
-      <c r="I26" s="45">
-        <v>0</v>
-      </c>
-      <c r="J26" s="45">
-        <v>20</v>
-      </c>
-      <c r="K26" s="45">
-        <v>1</v>
-      </c>
-      <c r="L26" s="45">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A27" s="45" t="s">
-        <v>139</v>
-      </c>
-      <c r="B27" s="45" t="s">
-        <v>82</v>
-      </c>
-      <c r="C27" s="45" t="s">
-        <v>123</v>
-      </c>
-      <c r="D27" s="45">
-        <v>0</v>
-      </c>
-      <c r="E27" s="45">
-        <v>0.57999999999999996</v>
-      </c>
-      <c r="F27" s="45">
-        <v>0.2</v>
-      </c>
-      <c r="G27" s="45">
-        <v>5000000</v>
-      </c>
-      <c r="H27" s="45">
-        <v>32000</v>
-      </c>
-      <c r="I27" s="45">
-        <v>26</v>
-      </c>
-      <c r="J27" s="45">
-        <v>15</v>
-      </c>
-      <c r="K27" s="45">
-        <v>1</v>
-      </c>
-      <c r="L27" s="45">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A28" s="45" t="s">
-        <v>140</v>
-      </c>
-      <c r="B28" s="45" t="s">
-        <v>82</v>
-      </c>
-      <c r="C28" s="45" t="s">
-        <v>4</v>
-      </c>
-      <c r="D28" s="45">
-        <v>0</v>
-      </c>
-      <c r="E28" s="45">
-        <v>0.45</v>
-      </c>
-      <c r="F28" s="45">
-        <v>0.44</v>
-      </c>
-      <c r="G28" s="45">
-        <v>1000000</v>
-      </c>
-      <c r="H28" s="45">
-        <v>10000</v>
-      </c>
-      <c r="I28" s="45">
-        <v>5.4</v>
-      </c>
-      <c r="J28" s="45">
-        <v>25</v>
-      </c>
-      <c r="K28" s="45">
-        <v>1</v>
-      </c>
-      <c r="L28" s="45">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A29" s="45" t="s">
-        <v>141</v>
-      </c>
-      <c r="B29" s="45" t="s">
-        <v>82</v>
-      </c>
-      <c r="C29" s="45" t="s">
-        <v>123</v>
-      </c>
-      <c r="D29" s="45">
-        <v>0</v>
-      </c>
-      <c r="E29" s="45">
-        <v>0.45</v>
-      </c>
-      <c r="F29" s="45">
-        <v>0.4</v>
-      </c>
-      <c r="G29" s="45">
-        <v>1000000</v>
-      </c>
-      <c r="H29" s="45">
-        <v>10000</v>
-      </c>
-      <c r="I29" s="45">
-        <v>8</v>
-      </c>
-      <c r="J29" s="45">
-        <v>25</v>
-      </c>
-      <c r="K29" s="45">
-        <v>1</v>
-      </c>
-      <c r="L29" s="45">
-        <v>0</v>
+      <c r="L29" s="44">
+        <v>0</v>
+      </c>
+      <c r="M29" s="44">
+        <v>100</v>
       </c>
     </row>
   </sheetData>
@@ -2228,7 +2315,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -2236,11 +2323,11 @@
         <v>13</v>
       </c>
       <c r="B2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="20" t="s">
+      <c r="A3" s="19" t="s">
         <v>2</v>
       </c>
       <c r="B3">
@@ -2286,72 +2373,72 @@
         <v>30</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="26" t="s">
+      <c r="A3" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="31" t="s">
+      <c r="B3" s="30" t="s">
         <v>35</v>
       </c>
-      <c r="C3" s="29">
+      <c r="C3" s="28">
         <v>0.8</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="26" t="s">
-        <v>123</v>
-      </c>
-      <c r="B4" s="28">
+      <c r="A4" s="25" t="s">
+        <v>121</v>
+      </c>
+      <c r="B4" s="27">
         <v>100</v>
       </c>
-      <c r="C4" s="29">
+      <c r="C4" s="28">
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="26" t="s">
-        <v>121</v>
-      </c>
-      <c r="B5" s="28">
+      <c r="A5" s="25" t="s">
+        <v>119</v>
+      </c>
+      <c r="B5" s="27">
         <v>55.4</v>
       </c>
-      <c r="C5" s="29">
+      <c r="C5" s="28">
         <v>0.28000000000000003</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="26" t="s">
+      <c r="A6" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="30">
+      <c r="B6" s="29">
         <v>29.8</v>
       </c>
-      <c r="C6" s="29">
+      <c r="C6" s="28">
         <v>0.2</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="26" t="s">
-        <v>122</v>
-      </c>
-      <c r="B7" s="28">
+      <c r="A7" s="25" t="s">
+        <v>120</v>
+      </c>
+      <c r="B7" s="27">
         <v>7.7</v>
       </c>
-      <c r="C7" s="29">
+      <c r="C7" s="28">
         <v>0.34</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="26" t="s">
+      <c r="A8" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="28">
+      <c r="B8" s="27">
         <v>1</v>
       </c>
-      <c r="C8" s="29">
+      <c r="C8" s="28">
         <v>0.05</v>
       </c>
     </row>
@@ -2378,90 +2465,90 @@
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="44" t="s">
-        <v>128</v>
-      </c>
-      <c r="B11" s="44">
+      <c r="A11" s="43" t="s">
+        <v>126</v>
+      </c>
+      <c r="B11" s="43">
         <v>62</v>
       </c>
-      <c r="C11" s="44">
+      <c r="C11" s="43">
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="44" t="s">
-        <v>129</v>
-      </c>
-      <c r="B12" s="44">
+      <c r="A12" s="43" t="s">
+        <v>127</v>
+      </c>
+      <c r="B12" s="43">
         <v>22</v>
       </c>
-      <c r="C12" s="44">
+      <c r="C12" s="43">
         <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="27" t="s">
+      <c r="A13" s="26" t="s">
         <v>38</v>
       </c>
-      <c r="B13" s="28">
-        <v>0</v>
-      </c>
-      <c r="C13" s="29">
+      <c r="B13" s="27">
+        <v>0</v>
+      </c>
+      <c r="C13" s="28">
         <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="39" t="s">
+      <c r="A14" s="38" t="s">
+        <v>122</v>
+      </c>
+      <c r="B14" s="27">
+        <v>0</v>
+      </c>
+      <c r="C14" s="28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="38" t="s">
+        <v>123</v>
+      </c>
+      <c r="B15" s="27">
+        <v>0</v>
+      </c>
+      <c r="C15" s="28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="38" t="s">
         <v>124</v>
       </c>
-      <c r="B14" s="28">
-        <v>0</v>
-      </c>
-      <c r="C14" s="29">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="39" t="s">
+      <c r="B16" s="41">
+        <v>0</v>
+      </c>
+      <c r="C16" s="42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="38" t="s">
         <v>125</v>
       </c>
-      <c r="B15" s="28">
-        <v>0</v>
-      </c>
-      <c r="C15" s="29">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="39" t="s">
-        <v>126</v>
-      </c>
-      <c r="B16" s="42">
-        <v>0</v>
-      </c>
-      <c r="C16" s="43">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="39" t="s">
-        <v>127</v>
-      </c>
-      <c r="B17" s="42">
-        <v>0</v>
-      </c>
-      <c r="C17" s="43">
+      <c r="B17" s="41">
+        <v>0</v>
+      </c>
+      <c r="C17" s="42">
         <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="39" t="s">
-        <v>143</v>
-      </c>
-      <c r="B18" s="42">
-        <v>0</v>
-      </c>
-      <c r="C18" s="43">
+      <c r="A18" s="38" t="s">
+        <v>141</v>
+      </c>
+      <c r="B18" s="41">
+        <v>0</v>
+      </c>
+      <c r="C18" s="42">
         <v>0</v>
       </c>
     </row>
@@ -2510,16 +2597,16 @@
     </row>
     <row r="2" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>45</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E2" s="6" t="s">
         <v>43</v>
@@ -2555,10 +2642,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:J3"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G27" sqref="G27"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2569,13 +2656,12 @@
     <col min="4" max="4" width="32" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="30.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="52.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="52.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>46</v>
       </c>
@@ -2583,7 +2669,7 @@
         <v>54</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D1" s="8" t="s">
         <v>50</v>
@@ -2595,19 +2681,16 @@
         <v>55</v>
       </c>
       <c r="G1" s="8" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="H1" s="8" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="I1" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="J1" s="8" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
         <v>13</v>
       </c>
@@ -2615,33 +2698,30 @@
         <v>51</v>
       </c>
       <c r="C2" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="G2" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="H2" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="I2" s="8" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
         <v>89</v>
-      </c>
-      <c r="D2" s="10" t="s">
-        <v>58</v>
-      </c>
-      <c r="E2" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="F2" s="8" t="s">
-        <v>60</v>
-      </c>
-      <c r="G2" s="8" t="s">
-        <v>61</v>
-      </c>
-      <c r="H2" s="8" t="s">
-        <v>87</v>
-      </c>
-      <c r="I2" s="8" t="s">
-        <v>90</v>
-      </c>
-      <c r="J2" s="8" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>91</v>
       </c>
       <c r="B3" s="3">
         <v>0</v>
@@ -2658,16 +2738,13 @@
       <c r="F3" s="3">
         <v>0.95</v>
       </c>
-      <c r="G3" s="3">
-        <v>0.95</v>
-      </c>
-      <c r="H3" s="32">
+      <c r="G3" s="31">
         <v>5000</v>
       </c>
-      <c r="I3" s="32">
+      <c r="H3" s="31">
         <v>100</v>
       </c>
-      <c r="J3" s="3">
+      <c r="I3" s="3">
         <v>25</v>
       </c>
     </row>
@@ -2693,18 +2770,18 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
-        <v>109</v>
-      </c>
-      <c r="B1" s="19" t="s">
-        <v>99</v>
+        <v>107</v>
+      </c>
+      <c r="B1" s="18" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B2" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -2712,23 +2789,23 @@
         <v>0</v>
       </c>
       <c r="B3" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B4" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B5" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -2736,39 +2813,39 @@
         <v>1</v>
       </c>
       <c r="B6" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="11" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B7" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="11" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B8" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="11" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B9" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B10" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
   </sheetData>
@@ -2787,35 +2864,35 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="B2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C2" t="s">
         <v>65</v>
       </c>
-      <c r="B2" t="s">
+      <c r="D2" t="s">
         <v>66</v>
       </c>
-      <c r="C2" t="s">
+      <c r="E2" t="s">
         <v>67</v>
       </c>
-      <c r="D2" t="s">
+      <c r="F2" t="s">
         <v>68</v>
       </c>
-      <c r="E2" t="s">
+      <c r="G2" t="s">
         <v>69</v>
-      </c>
-      <c r="F2" t="s">
-        <v>70</v>
-      </c>
-      <c r="G2" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B3">
         <v>48.67</v>
@@ -2838,7 +2915,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B4">
         <v>40.96</v>
@@ -2861,7 +2938,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B5">
         <v>23.95</v>
@@ -2884,7 +2961,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -2907,7 +2984,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B7">
         <v>0</v>
@@ -2930,7 +3007,7 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B8">
         <v>0</v>
@@ -2953,7 +3030,7 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B9">
         <v>0</v>
@@ -2989,35 +3066,35 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="B2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C2" t="s">
         <v>65</v>
       </c>
-      <c r="B2" t="s">
+      <c r="D2" t="s">
         <v>66</v>
       </c>
-      <c r="C2" t="s">
+      <c r="E2" t="s">
         <v>67</v>
       </c>
-      <c r="D2" t="s">
+      <c r="F2" t="s">
         <v>68</v>
       </c>
-      <c r="E2" t="s">
+      <c r="G2" t="s">
         <v>69</v>
-      </c>
-      <c r="F2" t="s">
-        <v>70</v>
-      </c>
-      <c r="G2" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B3">
         <v>5.01</v>
@@ -3040,7 +3117,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B4">
         <v>4.76</v>
@@ -3063,7 +3140,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B5">
         <v>4.6399999999999997</v>
@@ -3086,7 +3163,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -3109,7 +3186,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B7">
         <v>0</v>
@@ -3132,7 +3209,7 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B8">
         <v>0</v>
@@ -3155,7 +3232,7 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B9">
         <v>0</v>
@@ -3191,35 +3268,35 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C2" t="s">
         <v>65</v>
       </c>
-      <c r="B2" t="s">
+      <c r="D2" t="s">
         <v>66</v>
       </c>
-      <c r="C2" t="s">
+      <c r="E2" t="s">
         <v>67</v>
       </c>
-      <c r="D2" t="s">
+      <c r="F2" t="s">
         <v>68</v>
       </c>
-      <c r="E2" t="s">
+      <c r="G2" t="s">
         <v>69</v>
-      </c>
-      <c r="F2" t="s">
-        <v>70</v>
-      </c>
-      <c r="G2" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B3">
         <v>3.08</v>
@@ -3242,7 +3319,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B4">
         <v>2.99</v>
@@ -3265,7 +3342,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B5">
         <v>2.94</v>
@@ -3288,7 +3365,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -3311,7 +3388,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B7">
         <v>0</v>
@@ -3334,7 +3411,7 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B8">
         <v>0</v>
@@ -3357,7 +3434,7 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B9">
         <v>0</v>
@@ -3395,35 +3472,35 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C2" t="s">
         <v>65</v>
       </c>
-      <c r="B2" t="s">
+      <c r="D2" t="s">
         <v>66</v>
       </c>
-      <c r="C2" t="s">
+      <c r="E2" t="s">
         <v>67</v>
       </c>
-      <c r="D2" t="s">
+      <c r="F2" t="s">
         <v>68</v>
       </c>
-      <c r="E2" t="s">
+      <c r="G2" t="s">
         <v>69</v>
-      </c>
-      <c r="F2" t="s">
-        <v>70</v>
-      </c>
-      <c r="G2" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B3">
         <v>3.41</v>
@@ -3446,7 +3523,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B4">
         <v>3.32</v>
@@ -3469,7 +3546,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B5">
         <v>3.26</v>
@@ -3492,7 +3569,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -3515,7 +3592,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B7">
         <v>0</v>
@@ -3538,7 +3615,7 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B8">
         <v>0</v>
@@ -3561,7 +3638,7 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B9">
         <v>0</v>

</xml_diff>

<commit_message>
add Pmax_el in Condensing mode for CHP_SE and some bug fixis
</commit_message>
<xml_diff>
--- a/app/modules/common/AD/F16_input/DH_technology_cost.xlsx
+++ b/app/modules/common/AD/F16_input/DH_technology_cost.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hasani\Documents\Workplace\Dispatch\app\modules\common\AD\F16_input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20840857-490B-4C80-8878-38248B7BD61C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F540B1C0-D4DC-4CA5-9CD7-02F630FB4087}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="10350" windowWidth="11970" windowHeight="4815" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="146">
   <si>
     <t>boiler</t>
   </si>
@@ -359,9 +359,6 @@
     <t>CHP-SE#Default</t>
   </si>
   <si>
-    <t>Pmax</t>
-  </si>
-  <si>
     <t>heat pump # Heat Pump (River 10°C)</t>
   </si>
   <si>
@@ -462,6 +459,15 @@
   </si>
   <si>
     <t>Ramping Costs [EUR/MWh]</t>
+  </si>
+  <si>
+    <t>P_max_el_j</t>
+  </si>
+  <si>
+    <t>Pmax_el</t>
+  </si>
+  <si>
+    <t>P_max in condensing mode [MWel]</t>
   </si>
 </sst>
 </file>
@@ -604,7 +610,7 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
@@ -729,6 +735,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Eingabe" xfId="3" builtinId="20"/>
@@ -1073,7 +1083,7 @@
   <dimension ref="A1:N29"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="K43" sqref="K43"/>
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1133,10 +1143,13 @@
         <v>60</v>
       </c>
       <c r="M1" s="39" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+        <v>141</v>
+      </c>
+      <c r="N1" s="5" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" s="7" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
         <v>13</v>
       </c>
@@ -1174,7 +1187,10 @@
         <v>61</v>
       </c>
       <c r="M2" s="39" t="s">
-        <v>143</v>
+        <v>142</v>
+      </c>
+      <c r="N2" s="7" t="s">
+        <v>145</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
@@ -1217,7 +1233,9 @@
       <c r="M3" s="39">
         <v>0</v>
       </c>
-      <c r="N3"/>
+      <c r="N3" s="22">
+        <v>0</v>
+      </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="20" t="s">
@@ -1259,7 +1277,9 @@
       <c r="M4" s="39">
         <v>0</v>
       </c>
-      <c r="N4"/>
+      <c r="N4" s="22">
+        <v>0</v>
+      </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="20" t="s">
@@ -1301,7 +1321,9 @@
       <c r="M5" s="39">
         <v>0</v>
       </c>
-      <c r="N5"/>
+      <c r="N5" s="22">
+        <v>0</v>
+      </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="20" t="s">
@@ -1343,7 +1365,9 @@
       <c r="M6" s="39">
         <v>0</v>
       </c>
-      <c r="N6"/>
+      <c r="N6" s="22">
+        <v>0</v>
+      </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="20" t="s">
@@ -1385,7 +1409,9 @@
       <c r="M7" s="39">
         <v>0</v>
       </c>
-      <c r="N7"/>
+      <c r="N7" s="22">
+        <v>0</v>
+      </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="20" t="s">
@@ -1427,7 +1453,9 @@
       <c r="M8" s="39">
         <v>0</v>
       </c>
-      <c r="N8"/>
+      <c r="N8" s="22">
+        <v>0</v>
+      </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="20" t="s">
@@ -1469,11 +1497,13 @@
       <c r="M9" s="39">
         <v>0</v>
       </c>
-      <c r="N9"/>
+      <c r="N9" s="22">
+        <v>0</v>
+      </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="20" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B10" s="20" t="s">
         <v>81</v>
@@ -1511,7 +1541,9 @@
       <c r="M10" s="39">
         <v>100</v>
       </c>
-      <c r="N10"/>
+      <c r="N10" s="22">
+        <v>0</v>
+      </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="20" t="s">
@@ -1553,7 +1585,9 @@
       <c r="M11" s="39">
         <v>100</v>
       </c>
-      <c r="N11"/>
+      <c r="N11" s="22">
+        <v>0</v>
+      </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="20" t="s">
@@ -1595,10 +1629,13 @@
       <c r="M12" s="39">
         <v>100</v>
       </c>
+      <c r="N12" s="22">
+        <v>0</v>
+      </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="23" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B13" s="23" t="s">
         <v>56</v>
@@ -1636,10 +1673,13 @@
       <c r="M13" s="39">
         <v>0</v>
       </c>
+      <c r="N13" s="22">
+        <v>0</v>
+      </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="16" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B14" s="16" t="s">
         <v>76</v>
@@ -1677,10 +1717,13 @@
       <c r="M14" s="39">
         <v>0</v>
       </c>
+      <c r="N14" s="22">
+        <v>0</v>
+      </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="16" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B15" s="16" t="s">
         <v>76</v>
@@ -1718,11 +1761,13 @@
       <c r="M15" s="39">
         <v>0</v>
       </c>
-      <c r="N15"/>
+      <c r="N15" s="22">
+        <v>0</v>
+      </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="16" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B16" s="16" t="s">
         <v>76</v>
@@ -1760,11 +1805,13 @@
       <c r="M16" s="39">
         <v>0</v>
       </c>
-      <c r="N16"/>
+      <c r="N16" s="22">
+        <v>0</v>
+      </c>
     </row>
     <row r="17" spans="1:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="16" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B17" s="16" t="s">
         <v>76</v>
@@ -1802,11 +1849,13 @@
       <c r="M17" s="39">
         <v>0</v>
       </c>
-      <c r="N17"/>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N17" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="44" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B18" s="44" t="s">
         <v>1</v>
@@ -1844,11 +1893,13 @@
       <c r="M18" s="44">
         <v>100</v>
       </c>
-      <c r="N18"/>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N18" s="46">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="44" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B19" s="44" t="s">
         <v>77</v>
@@ -1886,16 +1937,19 @@
       <c r="M19" s="44">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N19" s="46">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="44" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B20" s="44" t="s">
         <v>78</v>
       </c>
       <c r="C20" s="44" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D20" s="44">
         <v>0</v>
@@ -1927,16 +1981,19 @@
       <c r="M20" s="44">
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N20" s="46">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="44" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B21" s="44" t="s">
         <v>79</v>
       </c>
       <c r="C21" s="44" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D21" s="44">
         <v>0</v>
@@ -1968,10 +2025,13 @@
       <c r="M21" s="44">
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N21" s="46">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="44" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B22" s="44" t="s">
         <v>81</v>
@@ -2009,10 +2069,13 @@
       <c r="M22" s="44">
         <v>100</v>
       </c>
-    </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N22" s="46">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="44" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B23" s="44" t="s">
         <v>81</v>
@@ -2050,10 +2113,13 @@
       <c r="M23" s="44">
         <v>100</v>
       </c>
-    </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N23" s="46">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="44" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B24" s="44" t="s">
         <v>81</v>
@@ -2091,10 +2157,13 @@
       <c r="M24" s="44">
         <v>100</v>
       </c>
-    </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N24" s="46">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="44" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B25" s="44" t="s">
         <v>81</v>
@@ -2132,10 +2201,13 @@
       <c r="M25" s="44">
         <v>100</v>
       </c>
-    </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N25" s="46">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="44" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B26" s="44" t="s">
         <v>81</v>
@@ -2173,16 +2245,19 @@
       <c r="M26" s="44">
         <v>100</v>
       </c>
-    </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N26" s="46">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="44" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B27" s="44" t="s">
         <v>80</v>
       </c>
       <c r="C27" s="44" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D27" s="44">
         <v>0</v>
@@ -2214,10 +2289,13 @@
       <c r="M27" s="44">
         <v>100</v>
       </c>
-    </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N27" s="46">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="44" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B28" s="44" t="s">
         <v>80</v>
@@ -2255,16 +2333,19 @@
       <c r="M28" s="44">
         <v>100</v>
       </c>
-    </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N28" s="46">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="44" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B29" s="44" t="s">
         <v>80</v>
       </c>
       <c r="C29" s="44" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D29" s="44">
         <v>0</v>
@@ -2295,6 +2376,9 @@
       </c>
       <c r="M29" s="44">
         <v>100</v>
+      </c>
+      <c r="N29" s="46">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -2308,7 +2392,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H24" sqref="H24"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2323,7 +2407,7 @@
         <v>13</v>
       </c>
       <c r="B2" t="s">
-        <v>109</v>
+        <v>144</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -2389,7 +2473,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="25" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B4" s="27">
         <v>100</v>
@@ -2400,7 +2484,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="25" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B5" s="27">
         <v>55.4</v>
@@ -2422,7 +2506,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="25" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B7" s="27">
         <v>7.7</v>
@@ -2466,7 +2550,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="43" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B11" s="43">
         <v>62</v>
@@ -2477,7 +2561,7 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="43" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B12" s="43">
         <v>22</v>
@@ -2499,7 +2583,7 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="38" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B14" s="27">
         <v>0</v>
@@ -2510,7 +2594,7 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="38" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B15" s="27">
         <v>0</v>
@@ -2521,7 +2605,7 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="38" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B16" s="41">
         <v>0</v>
@@ -2532,7 +2616,7 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="38" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B17" s="41">
         <v>0</v>
@@ -2543,7 +2627,7 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="38" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B18" s="41">
         <v>0</v>
@@ -2864,7 +2948,7 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -3066,7 +3150,7 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -3268,7 +3352,7 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -3472,7 +3556,7 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
update  dh technology xlsx
</commit_message>
<xml_diff>
--- a/app/modules/common/AD/F16_input/DH_technology_cost.xlsx
+++ b/app/modules/common/AD/F16_input/DH_technology_cost.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20346"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20368"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hasani\Documents\Workplace\Dispatch\app\modules\common\AD\F16_input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F540B1C0-D4DC-4CA5-9CD7-02F630FB4087}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E5DA86A-CFD6-46AD-960F-E9D02589D909}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="10350" windowWidth="11970" windowHeight="4815" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1083,7 +1083,7 @@
   <dimension ref="A1:N29"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+      <selection activeCell="I35" sqref="I35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1269,7 +1269,7 @@
         <v>20</v>
       </c>
       <c r="K4" s="21">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L4" s="20">
         <v>0</v>
@@ -1313,7 +1313,7 @@
         <v>20</v>
       </c>
       <c r="K5" s="21">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L5" s="20">
         <v>0</v>
@@ -1357,7 +1357,7 @@
         <v>20</v>
       </c>
       <c r="K6" s="21">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L6" s="20">
         <v>0</v>
@@ -1401,7 +1401,7 @@
         <v>20</v>
       </c>
       <c r="K7" s="21">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="L7" s="20">
         <v>0</v>
@@ -1445,7 +1445,7 @@
         <v>20</v>
       </c>
       <c r="K8" s="21">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="L8" s="20">
         <v>0</v>
@@ -1489,7 +1489,7 @@
         <v>30</v>
       </c>
       <c r="K9" s="21">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L9" s="20">
         <v>0</v>
@@ -1665,7 +1665,7 @@
         <v>20</v>
       </c>
       <c r="K13" s="23">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L13" s="24">
         <v>0</v>
@@ -1709,7 +1709,7 @@
         <v>25</v>
       </c>
       <c r="K14" s="33">
-        <v>0.75</v>
+        <v>0</v>
       </c>
       <c r="L14" s="32">
         <v>0</v>
@@ -1753,7 +1753,7 @@
         <v>25</v>
       </c>
       <c r="K15" s="35">
-        <v>0.75</v>
+        <v>0</v>
       </c>
       <c r="L15" s="34">
         <v>0</v>
@@ -1797,7 +1797,7 @@
         <v>25</v>
       </c>
       <c r="K16" s="37">
-        <v>0.75</v>
+        <v>0</v>
       </c>
       <c r="L16" s="36">
         <v>0</v>
@@ -1841,7 +1841,7 @@
         <v>25</v>
       </c>
       <c r="K17" s="40">
-        <v>0.75</v>
+        <v>0</v>
       </c>
       <c r="L17" s="39">
         <v>0</v>
@@ -2061,7 +2061,7 @@
         <v>30</v>
       </c>
       <c r="K22" s="44">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L22" s="44">
         <v>0</v>
@@ -2105,7 +2105,7 @@
         <v>20</v>
       </c>
       <c r="K23" s="44">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L23" s="44">
         <v>0</v>
@@ -2149,7 +2149,7 @@
         <v>25</v>
       </c>
       <c r="K24" s="44">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L24" s="44">
         <v>0</v>
@@ -2193,7 +2193,7 @@
         <v>20</v>
       </c>
       <c r="K25" s="44">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L25" s="44">
         <v>0</v>
@@ -2237,7 +2237,7 @@
         <v>20</v>
       </c>
       <c r="K26" s="44">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L26" s="44">
         <v>0</v>
@@ -2281,7 +2281,7 @@
         <v>15</v>
       </c>
       <c r="K27" s="44">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L27" s="44">
         <v>0</v>
@@ -2325,7 +2325,7 @@
         <v>25</v>
       </c>
       <c r="K28" s="44">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L28" s="44">
         <v>0</v>
@@ -2369,7 +2369,7 @@
         <v>25</v>
       </c>
       <c r="K29" s="44">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L29" s="44">
         <v>0</v>
@@ -2646,7 +2646,7 @@
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2704,7 +2704,7 @@
         <v>25</v>
       </c>
       <c r="B3" s="2">
-        <v>0.5</v>
+        <v>0.05</v>
       </c>
       <c r="C3" s="2">
         <v>-20</v>
@@ -2729,7 +2729,7 @@
   <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="D15" sqref="D15:D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
update default storage losses to 0.01%
</commit_message>
<xml_diff>
--- a/app/modules/common/AD/F16_input/DH_technology_cost.xlsx
+++ b/app/modules/common/AD/F16_input/DH_technology_cost.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20368"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20373"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hasani\Documents\Workplace\Dispatch\app\modules\common\AD\F16_input\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hasani\Documents\Workplace\Dispatch Guide\Dispatch\app\modules\common\AD\F16_input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E5DA86A-CFD6-46AD-960F-E9D02589D909}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7856CDCC-EB18-46B1-8BB0-7475DA444C73}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="10350" windowWidth="11970" windowHeight="4815" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1083,7 +1083,7 @@
   <dimension ref="A1:N29"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="I35" sqref="I35"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2392,10 +2392,14 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="37.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.5703125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -2729,7 +2733,7 @@
   <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D15" sqref="D15:D16"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2811,7 +2815,7 @@
         <v>0</v>
       </c>
       <c r="C3" s="3">
-        <v>1</v>
+        <v>0.01</v>
       </c>
       <c r="D3" s="3">
         <v>0</v>
@@ -2843,7 +2847,7 @@
   <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:A10"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>